<commit_message>
Tried to fix logistic regression result
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -40,13 +40,16 @@
     <t xml:space="preserve">F1</t>
   </si>
   <si>
+    <t xml:space="preserve">Logistic Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multinomial Naive Bayes</t>
   </si>
   <si>
     <t xml:space="preserve">Support Vector Machines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logistic Regression</t>
   </si>
   <si>
     <t xml:space="preserve">Decision Tree</t>
@@ -151,7 +154,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -185,25 +188,40 @@
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 5 models with only count vectorization results
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -43,10 +43,13 @@
     <t xml:space="preserve">Logistic Regression</t>
   </si>
   <si>
+    <t xml:space="preserve">Count Vectorizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multinomial Naive Bayes</t>
+  </si>
+  <si>
     <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multinomial Naive Bayes</t>
   </si>
   <si>
     <t xml:space="preserve">Support Vector Machines</t>
@@ -70,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,14 +158,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -191,37 +195,49 @@
       <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <v>82.46</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>92.86</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>88.32</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 5 models with count vectorizer and tfidf for Lucene
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Configuration</t>
   </si>
   <si>
+    <t xml:space="preserve">F1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accuracy</t>
   </si>
   <si>
@@ -37,9 +40,6 @@
     <t xml:space="preserve">Recall </t>
   </si>
   <si>
-    <t xml:space="preserve">F1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Logistic Regression</t>
   </si>
   <si>
@@ -49,9 +49,6 @@
     <t xml:space="preserve">Multinomial Naive Bayes</t>
   </si>
   <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Support Vector Machines</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Random Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf</t>
   </si>
 </sst>
 </file>
@@ -155,10 +155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -196,16 +196,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>88.32</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>82.46</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>84.42</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>92.86</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>88.32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -213,31 +213,179 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>88.01</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>81.11</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>80.4</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>97.45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>83.86</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>72.76</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>99.79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>82.76</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>93.76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>88.33</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>82.09</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>83.02</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>94.55</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C7" s="0" t="n">
+        <v>88.91</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>79.75</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>81.43</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>82.64</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>93.96</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>88.23</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>81.96</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>83.04</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>94.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 5 models with count vectorization, tfidf, 3-grams
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3)</t>
   </si>
 </sst>
 </file>
@@ -155,10 +164,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -388,6 +397,306 @@
         <v>94.37</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>88.91</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>79.57</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>88.55</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>82.58</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>83.43</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>94.59</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>88.37</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>82.25</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>83.41</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>94.22</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>88.75</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>82.13</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>80.63</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>98.96</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>88.19</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>80.99</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>79.25</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>99.72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>87.78</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>81.39</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>82.87</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>87.76</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>82.61</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>93.78</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>80.06</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>99.06</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>88.07</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>80.74</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>78.98</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>99.82</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>87.36</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>80.66</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>82.34</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>87.54</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>81.02</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>82.48</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>93.5</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Top 5 models with previous experiments plus SMOTE oversampling
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + SMOTE</t>
   </si>
 </sst>
 </file>
@@ -164,16 +167,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8979591836735"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
@@ -695,6 +698,106 @@
       </c>
       <c r="F26" s="0" t="n">
         <v>93.5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>88.47</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>83.97</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>88.35</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>92.77</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>87.98</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>80.58</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>78.89</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>73.21</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>82.51</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>79.57</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>86.95</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>80.41</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>83.02</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>91.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 5 models with Random Under Sampling for Lucene
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + SMOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + RUS</t>
   </si>
 </sst>
 </file>
@@ -167,10 +170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -800,6 +803,106 @@
         <v>91.48</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>88.81</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>83.34</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>85.39</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>86.29</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>80.37</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>86.27</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>86.42</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>87.81</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>80.25</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>78.53</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>69.42</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>62.01</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>83.55</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>59.68</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>69.61</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>71.79</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Top 5 models, combining Random Under Sampling + SMOTE and vice versa
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="20">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + RUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + RUS + SMOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + SMOTE + RUS</t>
   </si>
 </sst>
 </file>
@@ -170,10 +176,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -903,6 +909,206 @@
         <v>71.79</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>88.48</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>82.91</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>84.93</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>92.51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>86.61</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>80.94</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>86.66</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>86.79</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>87.89</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>80.41</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>78.69</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>69.54</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>62.62</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>59.74</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>79.4</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>72.43</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>86.34</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>73.87</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>82.74</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>84.12</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>93.56</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>82.99</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>84.68</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>92.82</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>87.93</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>78.84</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>99.73</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>81.86</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>74.07</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>82.52</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>81.49</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>87.26</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>80.78</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>92.15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Top 5 models with stop word inclusion
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="22">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + SMOTE + RUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + RUS + SMOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + SMOTE + RUS</t>
   </si>
 </sst>
 </file>
@@ -176,16 +182,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7551020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
@@ -1107,6 +1113,206 @@
       </c>
       <c r="F46" s="0" t="n">
         <v>92.15</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>86.4</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>80.12</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>84.93</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>88.06</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>81.78</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>75.58</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>88.12</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>87.95</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>80.86</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>79.79</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>98.21</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>60.14</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>56.24</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>46.09</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>70.86</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>65.49</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>89.33</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>58.97</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>87.76</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>81.84</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>85.16</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>90.71</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>86.61</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>80.78</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>86.63</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>86.66</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>87.95</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>80.99</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>80.27</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>97.46</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>78.58</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>71.49</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>85.94</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>72.62</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>80.56</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>73.95</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>86.74</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>75.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 5 models results with lemmatization for Lucene
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + SMOTE + RUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + lem + RUS + SMOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + lem + SMOTE + RUS</t>
   </si>
 </sst>
 </file>
@@ -182,16 +188,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0663265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
@@ -1313,6 +1319,206 @@
       </c>
       <c r="F56" s="0" t="n">
         <v>75.48</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>86.16</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>79.96</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>85.47</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>84.34</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>78.49</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>88.01</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>81.21</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>87.49</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>79.88</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>98.86</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>69.88</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>88.26</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>58.07</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>70.94</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>64.42</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>86.66</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>60.54</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>87.77</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>85.62</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>90.21</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>87.85</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>82.17</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>85.64</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>90.32</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>87.23</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>78.08</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>99.31</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>74.69</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>84.14</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>80.22</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>79.48</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>72.55</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>74.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 5 Models for Lucene with POS Tagging Feature
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="25">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + lem + SMOTE + RUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + POS</t>
   </si>
 </sst>
 </file>
@@ -188,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -221,504 +224,404 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>88.32</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>82.46</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>84.42</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>92.86</v>
-      </c>
-    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>88.01</v>
+        <v>88.32</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>81.11</v>
+        <v>82.46</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>80.4</v>
+        <v>84.42</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>97.45</v>
+        <v>92.86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>83.86</v>
+        <v>88.01</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>72.7</v>
+        <v>81.11</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>72.76</v>
+        <v>80.4</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>99.79</v>
+        <v>97.45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>87.8</v>
+        <v>83.86</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>81.35</v>
+        <v>72.7</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>82.76</v>
+        <v>72.76</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>93.76</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>88.33</v>
+        <v>87.8</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>82.09</v>
+        <v>81.35</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>83.02</v>
+        <v>82.76</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>94.55</v>
+        <v>93.76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>88.91</v>
+        <v>88.33</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>82.66</v>
+        <v>82.09</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>81.66</v>
+        <v>83.02</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>97.8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>88.44</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>81.48</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>79.75</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>99.54</v>
+        <v>94.55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>83.94</v>
+        <v>88.91</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>72.78</v>
+        <v>82.66</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>72.78</v>
+        <v>81.66</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>100</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>87.8</v>
+        <v>88.44</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>81.43</v>
+        <v>81.48</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>82.64</v>
+        <v>79.75</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>93.96</v>
+        <v>99.54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>88.23</v>
+        <v>83.94</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>81.96</v>
+        <v>72.78</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>83.04</v>
+        <v>72.78</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>94.37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>88.91</v>
+        <v>87.8</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>82.66</v>
+        <v>81.43</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>81.66</v>
+        <v>82.64</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>97.8</v>
+        <v>93.96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>88.44</v>
+        <v>88.23</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>81.48</v>
+        <v>81.96</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>79.57</v>
+        <v>83.04</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>99.54</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>83.94</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>72.78</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>72.78</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>100</v>
+        <v>94.37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>88.55</v>
+        <v>88.91</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>82.58</v>
+        <v>82.66</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>83.43</v>
+        <v>81.66</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>94.59</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>88.37</v>
+        <v>88.44</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>82.25</v>
+        <v>81.48</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>83.41</v>
+        <v>79.57</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>94.22</v>
+        <v>99.54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>88.75</v>
+        <v>83.94</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>82.13</v>
+        <v>72.78</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>80.63</v>
+        <v>72.78</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>98.96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>88.19</v>
+        <v>88.55</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>80.99</v>
+        <v>82.58</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>79.25</v>
+        <v>83.43</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>99.72</v>
+        <v>94.59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>83.94</v>
+        <v>88.37</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>72.78</v>
+        <v>82.25</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>72.78</v>
+        <v>83.41</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>87.78</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>81.39</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>82.87</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>93.6</v>
+        <v>94.22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>87.76</v>
+        <v>88.75</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>81.35</v>
+        <v>82.13</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>82.61</v>
+        <v>80.63</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>93.78</v>
+        <v>98.96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>88.44</v>
+        <v>88.19</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>81.56</v>
+        <v>80.99</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>80.06</v>
+        <v>79.25</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>99.06</v>
+        <v>99.72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>88.07</v>
+        <v>83.94</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>80.74</v>
+        <v>72.78</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>78.98</v>
+        <v>72.78</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>99.82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>83.94</v>
+        <v>87.78</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>72.78</v>
+        <v>81.39</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>72.78</v>
+        <v>82.87</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>100</v>
+        <v>93.6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>87.36</v>
+        <v>87.76</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>80.66</v>
+        <v>81.35</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>82.34</v>
+        <v>82.61</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>93.3</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>87.54</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>81.02</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>82.48</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>93.5</v>
+        <v>93.78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,19 +629,19 @@
         <v>6</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>88.47</v>
+        <v>88.44</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>82.66</v>
+        <v>81.56</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>83.97</v>
+        <v>80.06</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>93.6</v>
+        <v>99.06</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,19 +649,19 @@
         <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>88.35</v>
+        <v>88.07</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>82.66</v>
+        <v>80.74</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>84.42</v>
+        <v>78.98</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>92.77</v>
+        <v>99.82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,19 +669,19 @@
         <v>9</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>87.98</v>
+        <v>83.94</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>80.58</v>
+        <v>72.78</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>78.89</v>
+        <v>72.78</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>99.79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,19 +689,19 @@
         <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>80.95</v>
+        <v>87.36</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>73.21</v>
+        <v>80.66</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>82.51</v>
+        <v>82.34</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>79.57</v>
+        <v>93.3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,519 +709,419 @@
         <v>11</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>86.95</v>
+        <v>87.54</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>80.41</v>
+        <v>81.02</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>83.02</v>
+        <v>82.48</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>91.48</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>88.81</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>83.34</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>85.39</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>92.7</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>86.29</v>
+        <v>88.47</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>80.37</v>
+        <v>82.66</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>86.27</v>
+        <v>83.97</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>86.42</v>
+        <v>93.6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>87.81</v>
+        <v>88.35</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>80.25</v>
+        <v>82.66</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>78.53</v>
+        <v>84.42</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>99.89</v>
+        <v>92.77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>69.42</v>
+        <v>87.98</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>62.01</v>
+        <v>80.58</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>83.55</v>
+        <v>78.89</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>59.68</v>
+        <v>99.79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>77.2</v>
+        <v>80.95</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>69.61</v>
+        <v>73.21</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>84.2</v>
+        <v>82.51</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>71.79</v>
+        <v>79.57</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>88.48</v>
+        <v>86.95</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>82.91</v>
+        <v>80.41</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>84.93</v>
+        <v>83.02</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>92.51</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>86.61</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>80.94</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>86.66</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>86.79</v>
+        <v>91.48</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>87.89</v>
+        <v>88.81</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>80.41</v>
+        <v>83.34</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>78.69</v>
+        <v>85.39</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>99.89</v>
+        <v>92.7</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>69.54</v>
+        <v>86.29</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>62.62</v>
+        <v>80.37</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>83.8</v>
+        <v>86.27</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>59.74</v>
+        <v>86.42</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>79.4</v>
+        <v>87.81</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>72.43</v>
+        <v>80.25</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>86.34</v>
+        <v>78.53</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>73.87</v>
+        <v>99.89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>88.52</v>
+        <v>69.42</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>82.74</v>
+        <v>62.01</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>84.12</v>
+        <v>83.55</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>93.56</v>
+        <v>59.68</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>88.52</v>
+        <v>77.2</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>82.99</v>
+        <v>69.61</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>84.68</v>
+        <v>84.2</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>92.82</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>87.93</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>80.5</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>78.84</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>99.73</v>
+        <v>71.79</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>81.86</v>
+        <v>88.48</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>74.07</v>
+        <v>82.91</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>82.52</v>
+        <v>84.93</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>81.49</v>
+        <v>92.51</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>87.26</v>
+        <v>86.61</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>80.78</v>
+        <v>80.94</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>83.06</v>
+        <v>86.66</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>92.15</v>
+        <v>86.79</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>86.4</v>
+        <v>87.89</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>80.12</v>
+        <v>80.41</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>84.93</v>
+        <v>78.69</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>88.06</v>
+        <v>99.89</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>81.78</v>
+        <v>69.54</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>75.58</v>
+        <v>62.62</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>88.12</v>
+        <v>83.8</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>76.5</v>
+        <v>59.74</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>87.95</v>
+        <v>79.4</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>80.86</v>
+        <v>72.43</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>79.79</v>
+        <v>86.34</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>98.21</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>60.14</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>56.24</v>
-      </c>
-      <c r="E50" s="0" t="n">
-        <v>88.2</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>46.09</v>
+        <v>73.87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>70.86</v>
+        <v>88.52</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>65.49</v>
+        <v>82.74</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>89.33</v>
+        <v>84.12</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>58.97</v>
+        <v>93.56</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>87.76</v>
+        <v>88.52</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>81.84</v>
+        <v>82.99</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>85.16</v>
+        <v>84.68</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>90.71</v>
+        <v>92.82</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>86.61</v>
+        <v>87.93</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>80.78</v>
+        <v>80.5</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>86.63</v>
+        <v>78.84</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>86.66</v>
+        <v>99.73</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>87.95</v>
+        <v>81.86</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>80.99</v>
+        <v>74.07</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>80.27</v>
+        <v>82.52</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>97.46</v>
+        <v>81.49</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>78.58</v>
+        <v>87.26</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>71.49</v>
+        <v>80.78</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>85.94</v>
+        <v>83.06</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>72.62</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>80.56</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>73.95</v>
-      </c>
-      <c r="E56" s="0" t="n">
-        <v>86.74</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>75.48</v>
+        <v>92.15</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,19 +1129,19 @@
         <v>6</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>86.16</v>
+        <v>86.4</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>79.96</v>
+        <v>80.12</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>85.47</v>
+        <v>84.93</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>87.1</v>
+        <v>88.06</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,19 +1149,19 @@
         <v>8</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>84.34</v>
+        <v>81.78</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>78.49</v>
+        <v>75.58</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>88.01</v>
+        <v>88.12</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>81.21</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,19 +1169,19 @@
         <v>9</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>87.49</v>
+        <v>87.95</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>79.88</v>
+        <v>80.86</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>78.7</v>
+        <v>79.79</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>98.86</v>
+        <v>98.21</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,19 +1189,19 @@
         <v>10</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>69.88</v>
+        <v>60.14</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>63.89</v>
+        <v>56.24</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>88.26</v>
+        <v>88.2</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>58.07</v>
+        <v>46.09</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,119 +1209,419 @@
         <v>11</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>70.94</v>
+        <v>70.86</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>64.42</v>
+        <v>65.49</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>86.66</v>
+        <v>89.33</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>60.54</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" s="0" t="n">
-        <v>87.77</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="E62" s="0" t="n">
-        <v>85.62</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <v>90.21</v>
+        <v>58.97</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>87.85</v>
+        <v>87.76</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>82.17</v>
+        <v>81.84</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>85.64</v>
+        <v>85.16</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>90.32</v>
+        <v>90.71</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>87.23</v>
+        <v>86.61</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>79.31</v>
+        <v>80.78</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>78.08</v>
+        <v>86.63</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>99.31</v>
+        <v>86.66</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>82</v>
+        <v>87.95</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>74.69</v>
+        <v>80.99</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>84.14</v>
+        <v>80.27</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>80.22</v>
+        <v>97.46</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>78.58</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>71.49</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>85.94</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>72.62</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B67" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>80.56</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>73.95</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>86.74</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>75.48</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>86.16</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>79.96</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>85.47</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>84.34</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>78.49</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>88.01</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>81.21</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>87.49</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>79.88</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>98.86</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>69.88</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>88.26</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>58.07</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>70.94</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>64.42</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>86.66</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>60.54</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C75" s="0" t="n">
+        <v>87.77</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>85.62</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>90.21</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>87.85</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>82.17</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>85.64</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>90.32</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>87.23</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>78.08</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>99.31</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>74.69</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>84.14</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>80.22</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" s="0" t="n">
         <v>79.48</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D79" s="0" t="n">
         <v>72.55</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E79" s="0" t="n">
         <v>86.3</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F79" s="0" t="n">
         <v>74.14</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>88.39</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>81.43</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>79.88</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>99.27</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>88.18</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>99.93</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>87.17</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>80.82</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>83.68</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>91.15</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>87.52</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>81.51</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>84.6</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>90.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lucene models update with stopwords and lemmatization
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="29">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -70,6 +70,21 @@
     <t xml:space="preserve">CV + tfidf + ngram(3)</t>
   </si>
   <si>
+    <t xml:space="preserve">CV + tfidf + ngram(1) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(1) + stopwords + lemmatization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(2) + POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(1) + POS</t>
+  </si>
+  <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + SMOTE</t>
   </si>
   <si>
@@ -93,9 +108,6 @@
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + lem + SMOTE + RUS</t>
   </si>
-  <si>
-    <t xml:space="preserve">CV + tfidf + ngram(3) + POS</t>
-  </si>
 </sst>
 </file>
 
@@ -104,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -125,6 +137,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,8 +188,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,16 +214,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F86" activeCellId="0" sqref="F86"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
@@ -732,16 +755,16 @@
         <v>16</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>88.47</v>
+        <v>88.55</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>82.66</v>
+        <v>81.97</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>83.97</v>
+        <v>81.06</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>93.6</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,16 +775,16 @@
         <v>16</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>88.35</v>
+        <v>88.38</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>82.66</v>
+        <v>81.48</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>84.42</v>
+        <v>80.12</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>92.77</v>
+        <v>98.82</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,16 +795,16 @@
         <v>16</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>87.98</v>
+        <v>83.94</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>80.58</v>
+        <v>72.78</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>78.89</v>
+        <v>72.78</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>99.79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,16 +815,16 @@
         <v>16</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>80.95</v>
+        <v>87.01</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>73.21</v>
+        <v>80.43</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>82.51</v>
+        <v>83.06</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>79.57</v>
+        <v>91.56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,16 +835,16 @@
         <v>16</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>86.95</v>
+        <v>86.88</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>80.41</v>
+        <v>80.37</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>83.02</v>
+        <v>83.62</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>91.48</v>
+        <v>90.68</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,16 +855,16 @@
         <v>17</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>88.81</v>
+        <v>88.14</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>83.34</v>
+        <v>81.15</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>85.39</v>
+        <v>80.25</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>92.7</v>
+        <v>98.1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,16 +875,16 @@
         <v>17</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>86.29</v>
+        <v>87.43</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>80.37</v>
+        <v>79.64</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>86.27</v>
+        <v>78.19</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>86.42</v>
+        <v>99.55</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,16 +895,16 @@
         <v>17</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>87.81</v>
+        <v>83.94</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>80.25</v>
+        <v>72.78</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>78.53</v>
+        <v>72.78</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>99.89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,16 +915,16 @@
         <v>17</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>69.42</v>
+        <v>84.38</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>62.01</v>
+        <v>77.59</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>83.55</v>
+        <v>84.31</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>59.68</v>
+        <v>84.61</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,16 +935,16 @@
         <v>17</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>77.2</v>
+        <v>84.32</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>69.61</v>
+        <v>77.63</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>84.2</v>
+        <v>84.79</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>71.79</v>
+        <v>83.99</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,16 +955,16 @@
         <v>18</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>88.48</v>
+        <v>88.39</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>82.91</v>
+        <v>81.43</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>84.93</v>
+        <v>79.88</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>92.51</v>
+        <v>99.27</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,16 +975,16 @@
         <v>18</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>86.61</v>
+        <v>88.18</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>80.94</v>
+        <v>80.95</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>86.66</v>
+        <v>79.11</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>86.79</v>
+        <v>99.93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,16 +995,16 @@
         <v>18</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>87.89</v>
+        <v>83.94</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>80.41</v>
+        <v>72.78</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>78.69</v>
+        <v>72.78</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>99.89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,16 +1015,16 @@
         <v>18</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>69.54</v>
+        <v>87.17</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>62.62</v>
+        <v>80.82</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>83.8</v>
+        <v>83.68</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>59.74</v>
+        <v>91.15</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,16 +1035,16 @@
         <v>18</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>79.4</v>
+        <v>87.52</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>72.43</v>
+        <v>81.51</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>86.34</v>
+        <v>84.6</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>73.87</v>
+        <v>90.81</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,16 +1055,16 @@
         <v>19</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>88.52</v>
+        <v>88.6</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>82.74</v>
+        <v>81.8</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>84.12</v>
+        <v>80.24</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>93.56</v>
+        <v>99.22</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,16 +1075,16 @@
         <v>19</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>88.52</v>
+        <v>88.27</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>82.99</v>
+        <v>81.11</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>84.68</v>
+        <v>79.28</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>92.82</v>
+        <v>99.88</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,16 +1095,16 @@
         <v>19</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>87.93</v>
+        <v>83.94</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>80.5</v>
+        <v>72.78</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>78.84</v>
+        <v>72.78</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>99.73</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,16 +1115,16 @@
         <v>19</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>81.86</v>
+        <v>87.5</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>74.07</v>
+        <v>81.19</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>82.52</v>
+        <v>83.74</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>81.49</v>
+        <v>91.89</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,16 +1135,16 @@
         <v>19</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>87.26</v>
+        <v>87.66</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>80.78</v>
+        <v>81.23</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>83.06</v>
+        <v>83.12</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>92.15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,16 +1155,16 @@
         <v>20</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>86.4</v>
+        <v>88.86</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>80.12</v>
+        <v>82.46</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>84.93</v>
+        <v>81.34</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>88.06</v>
+        <v>98.17</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,16 +1175,16 @@
         <v>20</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>81.78</v>
+        <v>88.42</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>75.58</v>
+        <v>81.39</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>88.12</v>
+        <v>79.55</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>76.5</v>
+        <v>99.81</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,16 +1195,16 @@
         <v>20</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>87.95</v>
+        <v>83.94</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>80.86</v>
+        <v>72.78</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>79.79</v>
+        <v>72.78</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>98.21</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,16 +1215,16 @@
         <v>20</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>60.14</v>
+        <v>87.85</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>56.24</v>
+        <v>81.56</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>88.2</v>
+        <v>83.24</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>46.09</v>
+        <v>93.32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,416 +1235,1736 @@
         <v>20</v>
       </c>
       <c r="C61" s="0" t="n">
+        <v>87.67</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>83.05</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>93.04</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>88.47</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E63" s="1" t="n">
+        <v>83.97</v>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>88.35</v>
+      </c>
+      <c r="D64" s="1" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E64" s="1" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="F64" s="1" t="n">
+        <v>92.77</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>87.98</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>80.58</v>
+      </c>
+      <c r="E65" s="1" t="n">
+        <v>78.89</v>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>73.21</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>82.51</v>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>79.57</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>86.95</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <v>80.41</v>
+      </c>
+      <c r="E67" s="1" t="n">
+        <v>83.02</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>91.48</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="1" t="n">
+        <v>88.81</v>
+      </c>
+      <c r="D69" s="1" t="n">
+        <v>83.34</v>
+      </c>
+      <c r="E69" s="1" t="n">
+        <v>85.39</v>
+      </c>
+      <c r="F69" s="1" t="n">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>86.29</v>
+      </c>
+      <c r="D70" s="1" t="n">
+        <v>80.37</v>
+      </c>
+      <c r="E70" s="1" t="n">
+        <v>86.27</v>
+      </c>
+      <c r="F70" s="1" t="n">
+        <v>86.42</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>87.81</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>80.25</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <v>78.53</v>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>69.42</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>62.01</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>83.55</v>
+      </c>
+      <c r="F72" s="1" t="n">
+        <v>59.68</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="D73" s="1" t="n">
+        <v>69.61</v>
+      </c>
+      <c r="E73" s="1" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="F73" s="1" t="n">
+        <v>71.79</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>88.48</v>
+      </c>
+      <c r="D75" s="1" t="n">
+        <v>82.91</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>84.93</v>
+      </c>
+      <c r="F75" s="1" t="n">
+        <v>92.51</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>86.61</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>80.94</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>86.66</v>
+      </c>
+      <c r="F76" s="1" t="n">
+        <v>86.79</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>87.89</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>80.41</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>78.69</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>69.54</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>62.62</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <v>59.74</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>79.4</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>72.43</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>86.34</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <v>73.87</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>82.74</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>84.12</v>
+      </c>
+      <c r="F81" s="1" t="n">
+        <v>93.56</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="D82" s="1" t="n">
+        <v>82.99</v>
+      </c>
+      <c r="E82" s="1" t="n">
+        <v>84.68</v>
+      </c>
+      <c r="F82" s="1" t="n">
+        <v>92.82</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>87.93</v>
+      </c>
+      <c r="D83" s="1" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="E83" s="1" t="n">
+        <v>78.84</v>
+      </c>
+      <c r="F83" s="1" t="n">
+        <v>99.73</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>81.86</v>
+      </c>
+      <c r="D84" s="1" t="n">
+        <v>74.07</v>
+      </c>
+      <c r="E84" s="1" t="n">
+        <v>82.52</v>
+      </c>
+      <c r="F84" s="1" t="n">
+        <v>81.49</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>87.26</v>
+      </c>
+      <c r="D85" s="1" t="n">
+        <v>80.78</v>
+      </c>
+      <c r="E85" s="1" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="F85" s="1" t="n">
+        <v>92.15</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>86.4</v>
+      </c>
+      <c r="D87" s="1" t="n">
+        <v>80.12</v>
+      </c>
+      <c r="E87" s="1" t="n">
+        <v>84.93</v>
+      </c>
+      <c r="F87" s="1" t="n">
+        <v>88.06</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>81.78</v>
+      </c>
+      <c r="D88" s="1" t="n">
+        <v>75.58</v>
+      </c>
+      <c r="E88" s="1" t="n">
+        <v>88.12</v>
+      </c>
+      <c r="F88" s="1" t="n">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>87.95</v>
+      </c>
+      <c r="D89" s="1" t="n">
+        <v>80.86</v>
+      </c>
+      <c r="E89" s="1" t="n">
+        <v>79.79</v>
+      </c>
+      <c r="F89" s="1" t="n">
+        <v>98.21</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>60.14</v>
+      </c>
+      <c r="D90" s="1" t="n">
+        <v>56.24</v>
+      </c>
+      <c r="E90" s="1" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="F90" s="1" t="n">
+        <v>46.09</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="1" t="n">
         <v>70.86</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D91" s="1" t="n">
         <v>65.49</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E91" s="1" t="n">
         <v>89.33</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="F91" s="1" t="n">
         <v>58.97</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B93" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>87.76</v>
+      </c>
+      <c r="D93" s="1" t="n">
+        <v>81.84</v>
+      </c>
+      <c r="E93" s="1" t="n">
+        <v>85.16</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>90.71</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>86.61</v>
+      </c>
+      <c r="D94" s="1" t="n">
+        <v>80.78</v>
+      </c>
+      <c r="E94" s="1" t="n">
+        <v>86.63</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <v>86.66</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>87.95</v>
+      </c>
+      <c r="D95" s="1" t="n">
+        <v>80.99</v>
+      </c>
+      <c r="E95" s="1" t="n">
+        <v>80.27</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>97.46</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>78.58</v>
+      </c>
+      <c r="D96" s="1" t="n">
+        <v>71.49</v>
+      </c>
+      <c r="E96" s="1" t="n">
+        <v>85.94</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>72.62</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>80.56</v>
+      </c>
+      <c r="D97" s="1" t="n">
+        <v>73.95</v>
+      </c>
+      <c r="E97" s="1" t="n">
+        <v>86.74</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>75.48</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>86.16</v>
+      </c>
+      <c r="D99" s="1" t="n">
+        <v>79.96</v>
+      </c>
+      <c r="E99" s="1" t="n">
+        <v>85.47</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>84.34</v>
+      </c>
+      <c r="D100" s="1" t="n">
+        <v>78.49</v>
+      </c>
+      <c r="E100" s="1" t="n">
+        <v>88.01</v>
+      </c>
+      <c r="F100" s="1" t="n">
+        <v>81.21</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>87.49</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>79.88</v>
+      </c>
+      <c r="E101" s="1" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="F101" s="1" t="n">
+        <v>98.86</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C102" s="1" t="n">
+        <v>69.88</v>
+      </c>
+      <c r="D102" s="1" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="E102" s="1" t="n">
+        <v>88.26</v>
+      </c>
+      <c r="F102" s="1" t="n">
+        <v>58.07</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>70.94</v>
+      </c>
+      <c r="D103" s="1" t="n">
+        <v>64.42</v>
+      </c>
+      <c r="E103" s="1" t="n">
+        <v>86.66</v>
+      </c>
+      <c r="F103" s="1" t="n">
+        <v>60.54</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C105" s="1" t="n">
+        <v>87.77</v>
+      </c>
+      <c r="D105" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="E105" s="1" t="n">
+        <v>85.62</v>
+      </c>
+      <c r="F105" s="1" t="n">
+        <v>90.21</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C106" s="1" t="n">
+        <v>87.85</v>
+      </c>
+      <c r="D106" s="1" t="n">
+        <v>82.17</v>
+      </c>
+      <c r="E106" s="1" t="n">
+        <v>85.64</v>
+      </c>
+      <c r="F106" s="1" t="n">
+        <v>90.32</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C107" s="1" t="n">
+        <v>87.23</v>
+      </c>
+      <c r="D107" s="1" t="n">
+        <v>79.31</v>
+      </c>
+      <c r="E107" s="1" t="n">
+        <v>78.08</v>
+      </c>
+      <c r="F107" s="1" t="n">
+        <v>99.31</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="D108" s="1" t="n">
+        <v>74.69</v>
+      </c>
+      <c r="E108" s="1" t="n">
+        <v>84.14</v>
+      </c>
+      <c r="F108" s="1" t="n">
+        <v>80.22</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C109" s="1" t="n">
+        <v>79.48</v>
+      </c>
+      <c r="D109" s="1" t="n">
+        <v>72.55</v>
+      </c>
+      <c r="E109" s="1" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="F109" s="1" t="n">
+        <v>74.14</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C111" s="1" t="n">
+        <v>88.47</v>
+      </c>
+      <c r="D111" s="1" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E111" s="1" t="n">
+        <v>83.97</v>
+      </c>
+      <c r="F111" s="1" t="n">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" s="1" t="n">
+        <v>88.35</v>
+      </c>
+      <c r="D112" s="1" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E112" s="1" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="F112" s="1" t="n">
+        <v>92.77</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" s="1" t="n">
+        <v>87.98</v>
+      </c>
+      <c r="D113" s="1" t="n">
+        <v>80.58</v>
+      </c>
+      <c r="E113" s="1" t="n">
+        <v>78.89</v>
+      </c>
+      <c r="F113" s="1" t="n">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" s="1" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="D114" s="1" t="n">
+        <v>73.21</v>
+      </c>
+      <c r="E114" s="1" t="n">
+        <v>82.51</v>
+      </c>
+      <c r="F114" s="1" t="n">
+        <v>79.57</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115" s="1" t="n">
+        <v>86.95</v>
+      </c>
+      <c r="D115" s="1" t="n">
+        <v>80.41</v>
+      </c>
+      <c r="E115" s="1" t="n">
+        <v>83.02</v>
+      </c>
+      <c r="F115" s="1" t="n">
+        <v>91.48</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C117" s="1" t="n">
+        <v>88.81</v>
+      </c>
+      <c r="D117" s="1" t="n">
+        <v>83.34</v>
+      </c>
+      <c r="E117" s="1" t="n">
+        <v>85.39</v>
+      </c>
+      <c r="F117" s="1" t="n">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" s="1" t="n">
+        <v>86.29</v>
+      </c>
+      <c r="D118" s="1" t="n">
+        <v>80.37</v>
+      </c>
+      <c r="E118" s="1" t="n">
+        <v>86.27</v>
+      </c>
+      <c r="F118" s="1" t="n">
+        <v>86.42</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C119" s="1" t="n">
+        <v>87.81</v>
+      </c>
+      <c r="D119" s="1" t="n">
+        <v>80.25</v>
+      </c>
+      <c r="E119" s="1" t="n">
+        <v>78.53</v>
+      </c>
+      <c r="F119" s="1" t="n">
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120" s="1" t="n">
+        <v>69.42</v>
+      </c>
+      <c r="D120" s="1" t="n">
+        <v>62.01</v>
+      </c>
+      <c r="E120" s="1" t="n">
+        <v>83.55</v>
+      </c>
+      <c r="F120" s="1" t="n">
+        <v>59.68</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C121" s="1" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="D121" s="1" t="n">
+        <v>69.61</v>
+      </c>
+      <c r="E121" s="1" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="F121" s="1" t="n">
+        <v>71.79</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" s="1" t="n">
+        <v>88.48</v>
+      </c>
+      <c r="D123" s="1" t="n">
+        <v>82.91</v>
+      </c>
+      <c r="E123" s="1" t="n">
+        <v>84.93</v>
+      </c>
+      <c r="F123" s="1" t="n">
+        <v>92.51</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" s="1" t="n">
+        <v>86.61</v>
+      </c>
+      <c r="D124" s="1" t="n">
+        <v>80.94</v>
+      </c>
+      <c r="E124" s="1" t="n">
+        <v>86.66</v>
+      </c>
+      <c r="F124" s="1" t="n">
+        <v>86.79</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C125" s="1" t="n">
+        <v>87.89</v>
+      </c>
+      <c r="D125" s="1" t="n">
+        <v>80.41</v>
+      </c>
+      <c r="E125" s="1" t="n">
+        <v>78.69</v>
+      </c>
+      <c r="F125" s="1" t="n">
+        <v>99.89</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126" s="1" t="n">
+        <v>69.54</v>
+      </c>
+      <c r="D126" s="1" t="n">
+        <v>62.62</v>
+      </c>
+      <c r="E126" s="1" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="F126" s="1" t="n">
+        <v>59.74</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C127" s="1" t="n">
+        <v>79.4</v>
+      </c>
+      <c r="D127" s="1" t="n">
+        <v>72.43</v>
+      </c>
+      <c r="E127" s="1" t="n">
+        <v>86.34</v>
+      </c>
+      <c r="F127" s="1" t="n">
+        <v>73.87</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" s="1" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="D129" s="1" t="n">
+        <v>82.74</v>
+      </c>
+      <c r="E129" s="1" t="n">
+        <v>84.12</v>
+      </c>
+      <c r="F129" s="1" t="n">
+        <v>93.56</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C130" s="1" t="n">
+        <v>88.52</v>
+      </c>
+      <c r="D130" s="1" t="n">
+        <v>82.99</v>
+      </c>
+      <c r="E130" s="1" t="n">
+        <v>84.68</v>
+      </c>
+      <c r="F130" s="1" t="n">
+        <v>92.82</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C131" s="1" t="n">
+        <v>87.93</v>
+      </c>
+      <c r="D131" s="1" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="E131" s="1" t="n">
+        <v>78.84</v>
+      </c>
+      <c r="F131" s="1" t="n">
+        <v>99.73</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C132" s="1" t="n">
+        <v>81.86</v>
+      </c>
+      <c r="D132" s="1" t="n">
+        <v>74.07</v>
+      </c>
+      <c r="E132" s="1" t="n">
+        <v>82.52</v>
+      </c>
+      <c r="F132" s="1" t="n">
+        <v>81.49</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" s="1" t="n">
+        <v>87.26</v>
+      </c>
+      <c r="D133" s="1" t="n">
+        <v>80.78</v>
+      </c>
+      <c r="E133" s="1" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="F133" s="1" t="n">
+        <v>92.15</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C135" s="1" t="n">
+        <v>86.4</v>
+      </c>
+      <c r="D135" s="1" t="n">
+        <v>80.12</v>
+      </c>
+      <c r="E135" s="1" t="n">
+        <v>84.93</v>
+      </c>
+      <c r="F135" s="1" t="n">
+        <v>88.06</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" s="1" t="n">
+        <v>81.78</v>
+      </c>
+      <c r="D136" s="1" t="n">
+        <v>75.58</v>
+      </c>
+      <c r="E136" s="1" t="n">
+        <v>88.12</v>
+      </c>
+      <c r="F136" s="1" t="n">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C137" s="1" t="n">
+        <v>87.95</v>
+      </c>
+      <c r="D137" s="1" t="n">
+        <v>80.86</v>
+      </c>
+      <c r="E137" s="1" t="n">
+        <v>79.79</v>
+      </c>
+      <c r="F137" s="1" t="n">
+        <v>98.21</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C138" s="1" t="n">
+        <v>60.14</v>
+      </c>
+      <c r="D138" s="1" t="n">
+        <v>56.24</v>
+      </c>
+      <c r="E138" s="1" t="n">
+        <v>88.2</v>
+      </c>
+      <c r="F138" s="1" t="n">
+        <v>46.09</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" s="1" t="n">
+        <v>70.86</v>
+      </c>
+      <c r="D139" s="1" t="n">
+        <v>65.49</v>
+      </c>
+      <c r="E139" s="1" t="n">
+        <v>89.33</v>
+      </c>
+      <c r="F139" s="1" t="n">
+        <v>58.97</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C141" s="1" t="n">
         <v>87.76</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D141" s="1" t="n">
         <v>81.84</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E141" s="1" t="n">
         <v>85.16</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F141" s="1" t="n">
         <v>90.71</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C64" s="0" t="n">
+      <c r="B142" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C142" s="1" t="n">
         <v>86.61</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D142" s="1" t="n">
         <v>80.78</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E142" s="1" t="n">
         <v>86.63</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F142" s="1" t="n">
         <v>86.66</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C65" s="0" t="n">
+      <c r="B143" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C143" s="1" t="n">
         <v>87.95</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="D143" s="1" t="n">
         <v>80.99</v>
       </c>
-      <c r="E65" s="0" t="n">
+      <c r="E143" s="1" t="n">
         <v>80.27</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F143" s="1" t="n">
         <v>97.46</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" s="0" t="n">
+      <c r="B144" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C144" s="1" t="n">
         <v>78.58</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D144" s="1" t="n">
         <v>71.49</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E144" s="1" t="n">
         <v>85.94</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F144" s="1" t="n">
         <v>72.62</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C67" s="0" t="n">
+      <c r="B145" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C145" s="1" t="n">
         <v>80.56</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D145" s="1" t="n">
         <v>73.95</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E145" s="1" t="n">
         <v>86.74</v>
       </c>
-      <c r="F67" s="0" t="n">
+      <c r="F145" s="1" t="n">
         <v>75.48</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C69" s="0" t="n">
+      <c r="B147" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C147" s="1" t="n">
         <v>86.16</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D147" s="1" t="n">
         <v>79.96</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E147" s="1" t="n">
         <v>85.47</v>
       </c>
-      <c r="F69" s="0" t="n">
+      <c r="F147" s="1" t="n">
         <v>87.1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C70" s="0" t="n">
+      <c r="B148" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C148" s="1" t="n">
         <v>84.34</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D148" s="1" t="n">
         <v>78.49</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E148" s="1" t="n">
         <v>88.01</v>
       </c>
-      <c r="F70" s="0" t="n">
+      <c r="F148" s="1" t="n">
         <v>81.21</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C71" s="0" t="n">
+      <c r="B149" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C149" s="1" t="n">
         <v>87.49</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D149" s="1" t="n">
         <v>79.88</v>
       </c>
-      <c r="E71" s="0" t="n">
+      <c r="E149" s="1" t="n">
         <v>78.7</v>
       </c>
-      <c r="F71" s="0" t="n">
+      <c r="F149" s="1" t="n">
         <v>98.86</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B72" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C72" s="0" t="n">
+      <c r="B150" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C150" s="1" t="n">
         <v>69.88</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D150" s="1" t="n">
         <v>63.89</v>
       </c>
-      <c r="E72" s="0" t="n">
+      <c r="E150" s="1" t="n">
         <v>88.26</v>
       </c>
-      <c r="F72" s="0" t="n">
+      <c r="F150" s="1" t="n">
         <v>58.07</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" s="0" t="n">
+      <c r="B151" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C151" s="1" t="n">
         <v>70.94</v>
       </c>
-      <c r="D73" s="0" t="n">
+      <c r="D151" s="1" t="n">
         <v>64.42</v>
       </c>
-      <c r="E73" s="0" t="n">
+      <c r="E151" s="1" t="n">
         <v>86.66</v>
       </c>
-      <c r="F73" s="0" t="n">
+      <c r="F151" s="1" t="n">
         <v>60.54</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B75" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C75" s="0" t="n">
+      <c r="B153" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C153" s="1" t="n">
         <v>87.77</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D153" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="E75" s="0" t="n">
+      <c r="E153" s="1" t="n">
         <v>85.62</v>
       </c>
-      <c r="F75" s="0" t="n">
+      <c r="F153" s="1" t="n">
         <v>90.21</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76" s="0" t="n">
+      <c r="B154" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C154" s="1" t="n">
         <v>87.85</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D154" s="1" t="n">
         <v>82.17</v>
       </c>
-      <c r="E76" s="0" t="n">
+      <c r="E154" s="1" t="n">
         <v>85.64</v>
       </c>
-      <c r="F76" s="0" t="n">
+      <c r="F154" s="1" t="n">
         <v>90.32</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" s="0" t="n">
+      <c r="B155" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C155" s="1" t="n">
         <v>87.23</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D155" s="1" t="n">
         <v>79.31</v>
       </c>
-      <c r="E77" s="0" t="n">
+      <c r="E155" s="1" t="n">
         <v>78.08</v>
       </c>
-      <c r="F77" s="0" t="n">
+      <c r="F155" s="1" t="n">
         <v>99.31</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C78" s="0" t="n">
+      <c r="B156" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C156" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D156" s="1" t="n">
         <v>74.69</v>
       </c>
-      <c r="E78" s="0" t="n">
+      <c r="E156" s="1" t="n">
         <v>84.14</v>
       </c>
-      <c r="F78" s="0" t="n">
+      <c r="F156" s="1" t="n">
         <v>80.22</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C79" s="0" t="n">
+      <c r="B157" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C157" s="1" t="n">
         <v>79.48</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D157" s="1" t="n">
         <v>72.55</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E157" s="1" t="n">
         <v>86.3</v>
       </c>
-      <c r="F79" s="0" t="n">
+      <c r="F157" s="1" t="n">
         <v>74.14</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C81" s="0" t="n">
-        <v>88.39</v>
-      </c>
-      <c r="D81" s="0" t="n">
-        <v>81.43</v>
-      </c>
-      <c r="E81" s="0" t="n">
-        <v>79.88</v>
-      </c>
-      <c r="F81" s="0" t="n">
-        <v>99.27</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C82" s="0" t="n">
-        <v>88.18</v>
-      </c>
-      <c r="D82" s="0" t="n">
-        <v>80.95</v>
-      </c>
-      <c r="E82" s="0" t="n">
-        <v>79.11</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>99.93</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C83" s="0" t="n">
-        <v>83.94</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>72.78</v>
-      </c>
-      <c r="E83" s="0" t="n">
-        <v>72.78</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>87.17</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>80.82</v>
-      </c>
-      <c r="E84" s="0" t="n">
-        <v>83.68</v>
-      </c>
-      <c r="F84" s="0" t="n">
-        <v>91.15</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>87.52</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>81.51</v>
-      </c>
-      <c r="E85" s="0" t="n">
-        <v>84.6</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>90.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added template for Thunderbird and Ubuntu excel file
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ubuntu" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Thunderbird" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="29">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -216,15 +218,14 @@
   </sheetPr>
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2976,4 +2977,2102 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>88.32</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>82.46</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>92.86</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>88.01</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>81.11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>80.4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>97.45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>83.86</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>72.76</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>82.76</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>93.76</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>88.33</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>82.09</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>83.02</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>94.55</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>88.91</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>79.75</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>81.43</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>82.64</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>93.96</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>88.23</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>81.96</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>83.04</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>94.37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>88.91</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>79.57</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>88.55</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>82.58</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>83.43</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>94.59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>88.37</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>82.25</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>83.41</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>94.22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>88.75</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>82.13</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>80.63</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>98.96</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>88.19</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>80.99</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>79.25</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>99.72</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>87.78</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>81.39</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>82.87</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>87.76</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>82.61</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>93.78</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>80.06</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>99.06</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>88.07</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>80.74</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>78.98</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>99.82</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>87.36</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>80.66</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>82.34</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>87.54</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>81.02</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>82.48</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>88.55</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>81.97</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>81.06</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>88.38</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>80.12</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>98.82</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>87.01</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>80.43</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>91.56</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>86.88</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>80.37</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>83.62</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>90.68</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>88.14</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>81.15</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>80.25</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>87.43</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>79.64</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>78.19</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>99.55</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>84.38</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>77.59</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>84.31</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>84.61</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>84.32</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>77.63</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>84.79</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>83.99</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>88.39</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>81.43</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>79.88</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>99.27</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>88.18</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>99.93</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>87.17</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>80.82</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>83.68</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>91.15</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>87.52</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>81.51</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>84.6</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>90.81</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>88.6</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>80.24</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>99.22</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>88.27</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>81.11</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>79.28</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>99.88</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>81.19</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>83.74</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>91.89</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>87.66</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>81.23</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>83.12</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>88.86</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>82.46</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>81.34</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>98.17</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>88.42</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>81.39</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>99.81</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>87.85</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>83.24</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>93.32</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>87.67</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>83.05</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>93.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>88.32</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>82.46</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>84.42</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>92.86</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>88.01</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>81.11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>80.4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>97.45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>83.86</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>72.76</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>82.76</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>93.76</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>88.33</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>82.09</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>83.02</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>94.55</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>88.91</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>79.75</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>81.43</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>82.64</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>93.96</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>88.23</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>81.96</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>83.04</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>94.37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>88.91</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>82.66</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>81.66</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>79.57</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>88.55</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>82.58</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>83.43</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>94.59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>88.37</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>82.25</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>83.41</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>94.22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>88.75</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>82.13</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>80.63</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>98.96</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>88.19</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>80.99</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>79.25</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>99.72</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>87.78</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>81.39</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>82.87</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>87.76</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>82.61</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>93.78</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>88.44</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>80.06</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>99.06</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>88.07</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>80.74</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>78.98</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>99.82</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>87.36</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>80.66</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>82.34</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>87.54</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>81.02</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>82.48</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>88.55</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>81.97</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>81.06</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>88.38</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>81.48</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>80.12</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>98.82</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>87.01</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>80.43</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>83.06</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>91.56</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>86.88</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>80.37</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>83.62</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>90.68</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>88.14</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>81.15</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>80.25</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>98.1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>87.43</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>79.64</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>78.19</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>99.55</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>84.38</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>77.59</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>84.31</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>84.61</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>84.32</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>77.63</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>84.79</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>83.99</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>88.39</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>81.43</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>79.88</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>99.27</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>88.18</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>99.93</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>87.17</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>80.82</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>83.68</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>91.15</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>87.52</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>81.51</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>84.6</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>90.81</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>88.6</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>80.24</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>99.22</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>88.27</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>81.11</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>79.28</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>99.88</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>81.19</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>83.74</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>91.89</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>87.66</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>81.23</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>83.12</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>88.86</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>82.46</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>81.34</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>98.17</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>88.42</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>81.39</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>79.55</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>99.81</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>83.94</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>72.78</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>87.85</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>83.24</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>93.32</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>87.67</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>81.35</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>83.05</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>93.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated experiment results for top 5 models in Ubuntu comments
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -2986,8 +2986,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F50" activeCellId="0" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3025,16 +3025,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>88.32</v>
+        <v>72.64</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>82.46</v>
+        <v>74.76</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>84.42</v>
+        <v>76</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>92.86</v>
+        <v>70.15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,16 +3045,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>88.01</v>
+        <v>72.86</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>81.11</v>
+        <v>70.74</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>80.4</v>
+        <v>65.96</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>97.45</v>
+        <v>82.66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3065,16 +3065,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>83.86</v>
+        <v>10.54</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>72.7</v>
+        <v>53.37</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>72.76</v>
+        <v>77.16</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>99.79</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,16 +3085,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>87.8</v>
+        <v>67.34</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>81.35</v>
+        <v>71.06</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>82.76</v>
+        <v>74.01</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>93.76</v>
+        <v>62.15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3105,16 +3105,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>88.33</v>
+        <v>65.44</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>82.09</v>
+        <v>66.46</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>83.02</v>
+        <v>64.46</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>94.55</v>
+        <v>66.99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,16 +3125,16 @@
         <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>88.91</v>
+        <v>74.31</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>82.66</v>
+        <v>74.15</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>81.66</v>
+        <v>71.48</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>97.8</v>
+        <v>78.15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,16 +3145,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>88.44</v>
+        <v>72.92</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>81.48</v>
+        <v>71.78</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>79.75</v>
+        <v>67.83</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>99.54</v>
+        <v>80.17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,16 +3165,16 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,16 +3185,16 @@
         <v>12</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>87.8</v>
+        <v>68.55</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>81.43</v>
+        <v>71.27</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>82.64</v>
+        <v>72.71</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>93.96</v>
+        <v>65.07</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3205,16 +3205,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>88.23</v>
+        <v>67</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>81.96</v>
+        <v>68.54</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>83.04</v>
+        <v>67.82</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>94.37</v>
+        <v>66.52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,16 +3225,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>88.91</v>
+        <v>74.31</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>82.66</v>
+        <v>74.15</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>81.66</v>
+        <v>71.48</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>97.8</v>
+        <v>78.15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3245,16 +3245,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>88.44</v>
+        <v>72.92</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>81.48</v>
+        <v>71.78</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>79.57</v>
+        <v>67.83</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>99.54</v>
+        <v>80.17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,16 +3265,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3285,16 +3285,16 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>88.55</v>
+        <v>68.97</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>82.58</v>
+        <v>71.78</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>83.43</v>
+        <v>73.23</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>94.59</v>
+        <v>65.74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,16 +3305,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>88.37</v>
+        <v>68.55</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>82.25</v>
+        <v>71.27</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>83.41</v>
+        <v>72.71</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>94.22</v>
+        <v>65.07</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,16 +3325,16 @@
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>88.75</v>
+        <v>75.41</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>82.13</v>
+        <v>73.79</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>80.63</v>
+        <v>68.32</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>98.96</v>
+        <v>85.03</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,16 +3345,16 @@
         <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>88.19</v>
+        <v>74.07</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>80.99</v>
+        <v>72.5</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>79.25</v>
+        <v>68.13</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>99.72</v>
+        <v>82.53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,16 +3365,16 @@
         <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,16 +3385,16 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>87.78</v>
+        <v>65.23</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>81.39</v>
+        <v>70.41</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>82.87</v>
+        <v>75.62</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>93.6</v>
+        <v>57.79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3405,16 +3405,16 @@
         <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>87.76</v>
+        <v>62.96</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>81.35</v>
+        <v>68.69</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>82.61</v>
+        <v>73.57</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>93.78</v>
+        <v>55.62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,16 +3425,16 @@
         <v>15</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>88.44</v>
+        <v>75.83</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>81.56</v>
+        <v>73.54</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>80.06</v>
+        <v>67.19</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>99.06</v>
+        <v>87.8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3445,16 +3445,16 @@
         <v>15</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>88.07</v>
+        <v>74.24</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>80.74</v>
+        <v>72.64</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>78.98</v>
+        <v>68.28</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>99.82</v>
+        <v>82.63</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,16 +3465,16 @@
         <v>15</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3485,16 +3485,16 @@
         <v>15</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>87.36</v>
+        <v>61.61</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>80.66</v>
+        <v>68.58</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>82.34</v>
+        <v>75.07</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>93.3</v>
+        <v>52.59</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,16 +3505,16 @@
         <v>15</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>87.54</v>
+        <v>61.04</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>81.02</v>
+        <v>67.79</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>82.48</v>
+        <v>73.8</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>93.5</v>
+        <v>52.57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,16 +3525,16 @@
         <v>16</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>88.55</v>
+        <v>68.9</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>81.97</v>
+        <v>69.3</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>81.06</v>
+        <v>67.14</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>97.8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,16 +3545,16 @@
         <v>16</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>88.38</v>
+        <v>69.32</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>81.48</v>
+        <v>69.26</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>80.12</v>
+        <v>67.24</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>98.82</v>
+        <v>73.46</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,16 +3565,16 @@
         <v>16</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,16 +3585,16 @@
         <v>16</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>87.01</v>
+        <v>57.61</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>80.43</v>
+        <v>65.95</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>83.06</v>
+        <v>71.96</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>91.56</v>
+        <v>48.49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3605,16 +3605,16 @@
         <v>16</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>86.88</v>
+        <v>57.9</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>80.37</v>
+        <v>66.46</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>83.62</v>
+        <v>73.77</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>90.68</v>
+        <v>47.99</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3625,16 +3625,16 @@
         <v>17</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>88.14</v>
+        <v>70.59</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>81.15</v>
+        <v>71.38</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>80.25</v>
+        <v>70.03</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>98.1</v>
+        <v>72.15</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,16 +3645,16 @@
         <v>17</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>87.43</v>
+        <v>69.35</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>79.64</v>
+        <v>69.08</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>78.19</v>
+        <v>67.16</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>99.55</v>
+        <v>73.49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3665,16 +3665,16 @@
         <v>17</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3685,16 +3685,16 @@
         <v>17</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>84.38</v>
+        <v>58.43</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>77.59</v>
+        <v>66.35</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>84.31</v>
+        <v>72.66</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>84.61</v>
+        <v>49.51</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,16 +3705,16 @@
         <v>17</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>84.32</v>
+        <v>60.44</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>77.63</v>
+        <v>68</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>84.79</v>
+        <v>74.84</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>83.99</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3725,16 +3725,16 @@
         <v>18</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>88.39</v>
+        <v>75.03</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>81.43</v>
+        <v>72.71</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>79.88</v>
+        <v>66.75</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>99.27</v>
+        <v>86.7</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3745,16 +3745,16 @@
         <v>18</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>88.18</v>
+        <v>73.42</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>80.95</v>
+        <v>72.21</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>79.11</v>
+        <v>67.93</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>99.93</v>
+        <v>81.37</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,16 +3765,16 @@
         <v>18</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3785,16 +3785,16 @@
         <v>18</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>87.17</v>
+        <v>61.43</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>80.82</v>
+        <v>64.8</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>83.68</v>
+        <v>65.39</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>91.15</v>
+        <v>58.25</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3805,16 +3805,16 @@
         <v>18</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>87.52</v>
+        <v>61.88</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>81.51</v>
+        <v>69.15</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>84.6</v>
+        <v>76.8</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>90.81</v>
+        <v>52.38</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,16 +3825,16 @@
         <v>19</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>88.6</v>
+        <v>74.83</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>81.8</v>
+        <v>73.39</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>80.24</v>
+        <v>68.36</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>99.22</v>
+        <v>83.88</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3845,16 +3845,16 @@
         <v>19</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>88.27</v>
+        <v>73.25</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>81.11</v>
+        <v>71.81</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>79.28</v>
+        <v>67.51</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>99.88</v>
+        <v>81.59</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,16 +3865,16 @@
         <v>19</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3885,16 +3885,16 @@
         <v>19</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>87.5</v>
+        <v>61.39</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>81.19</v>
+        <v>64.52</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>83.74</v>
+        <v>64.57</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>91.89</v>
+        <v>58.85</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,16 +3905,16 @@
         <v>19</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>87.66</v>
+        <v>63.44</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>81.23</v>
+        <v>69.05</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>83.12</v>
+        <v>74.02</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>93</v>
+        <v>55.86</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3925,16 +3925,16 @@
         <v>20</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>88.86</v>
+        <v>75.95</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>82.46</v>
+        <v>74.83</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>81.34</v>
+        <v>71.93</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>98.17</v>
+        <v>79.1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,16 +3945,16 @@
         <v>20</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>88.42</v>
+        <v>73.37</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>81.39</v>
+        <v>71.99</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>79.55</v>
+        <v>67.56</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>99.81</v>
+        <v>81.59</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,16 +3965,16 @@
         <v>20</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>83.94</v>
+        <v>0</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>72.78</v>
+        <v>51.51</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>72.78</v>
+        <v>0</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,16 +3985,16 @@
         <v>20</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>87.85</v>
+        <v>69.14</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>81.56</v>
+        <v>72.06</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>83.24</v>
+        <v>75.07</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>93.32</v>
+        <v>64.86</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4005,16 +4005,16 @@
         <v>20</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>87.67</v>
+        <v>66.29</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>81.35</v>
+        <v>68.43</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>83.05</v>
+        <v>68.42</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>93.04</v>
+        <v>64.59</v>
       </c>
     </row>
   </sheetData>
@@ -4035,8 +4035,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4674,16 +4674,16 @@
         <v>17</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>88.14</v>
+        <v>63.17</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>81.15</v>
+        <v>64.9</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>80.25</v>
+        <v>65.12</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>98.1</v>
+        <v>62.96</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4694,16 +4694,16 @@
         <v>17</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>87.43</v>
+        <v>63.51</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>79.64</v>
+        <v>62.86</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>78.19</v>
+        <v>61.37</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>99.55</v>
+        <v>67.43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4714,16 +4714,16 @@
         <v>17</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4734,16 +4734,16 @@
         <v>17</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>84.38</v>
+        <v>55.3</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>77.59</v>
+        <v>62.25</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>84.31</v>
+        <v>65.74</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>84.61</v>
+        <v>48.64</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,16 +4754,16 @@
         <v>17</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>84.32</v>
+        <v>55.92</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>77.63</v>
+        <v>63.06</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>84.79</v>
+        <v>66.72</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>83.99</v>
+        <v>48.75</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated top 5 models results for Thunderbird Comments data
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -219,7 +219,7 @@
   <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F53 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2986,8 +2986,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F50" activeCellId="0" sqref="F50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F50" activeCellId="1" sqref="F53 F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4035,8 +4035,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F53" activeCellId="0" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4074,16 +4074,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>88.32</v>
+        <v>67.6</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>82.46</v>
+        <v>69.96</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>84.42</v>
+        <v>71.33</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>92.86</v>
+        <v>64.78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,16 +4094,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>88.01</v>
+        <v>69.78</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>81.11</v>
+        <v>66.07</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>80.4</v>
+        <v>61.68</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>97.45</v>
+        <v>81.58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4114,16 +4114,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>83.86</v>
+        <v>19.09</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>72.7</v>
+        <v>54.7</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>72.76</v>
+        <v>75.33</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>99.79</v>
+        <v>11.21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4134,16 +4134,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>87.8</v>
+        <v>62.35</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>81.35</v>
+        <v>64.84</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>82.76</v>
+        <v>65.17</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>93.76</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,16 +4154,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>88.33</v>
+        <v>58.54</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>82.09</v>
+        <v>64.64</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>83.02</v>
+        <v>68.92</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>94.55</v>
+        <v>51.89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4174,16 +4174,16 @@
         <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>88.91</v>
+        <v>68.18</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>82.66</v>
+        <v>68.59</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>81.66</v>
+        <v>67.47</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>97.8</v>
+        <v>70.03</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,16 +4194,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>88.44</v>
+        <v>68.31</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>81.48</v>
+        <v>66.75</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>79.75</v>
+        <v>64.22</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>99.54</v>
+        <v>74.4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4214,16 +4214,16 @@
         <v>12</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,16 +4234,16 @@
         <v>12</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>87.8</v>
+        <v>61.15</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>81.43</v>
+        <v>62.73</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>82.64</v>
+        <v>62.54</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>93.96</v>
+        <v>60.57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,16 +4254,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>88.23</v>
+        <v>61.97</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>81.96</v>
+        <v>65.71</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>83.04</v>
+        <v>68.02</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>94.37</v>
+        <v>57.73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,16 +4274,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>88.91</v>
+        <v>68.18</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>82.66</v>
+        <v>68.59</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>81.66</v>
+        <v>67.47</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>97.8</v>
+        <v>70.03</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4294,16 +4294,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>88.44</v>
+        <v>68.31</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>81.48</v>
+        <v>66.75</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>79.57</v>
+        <v>64.22</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>99.54</v>
+        <v>74.4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4314,16 +4314,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,16 +4334,16 @@
         <v>13</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>88.55</v>
+        <v>61.15</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>82.58</v>
+        <v>62.73</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>83.43</v>
+        <v>62.54</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>94.59</v>
+        <v>60.57</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4354,16 +4354,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>88.37</v>
+        <v>61.97</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>82.25</v>
+        <v>65.71</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>83.41</v>
+        <v>68.02</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>94.22</v>
+        <v>57.73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,16 +4374,16 @@
         <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>88.75</v>
+        <v>72.15</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>82.13</v>
+        <v>70.35</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>80.63</v>
+        <v>66.66</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>98.96</v>
+        <v>79.11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,16 +4394,16 @@
         <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>88.19</v>
+        <v>70.19</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>80.99</v>
+        <v>67.52</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>79.25</v>
+        <v>63.94</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>99.72</v>
+        <v>79.19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4414,16 +4414,16 @@
         <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4434,16 +4434,16 @@
         <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>87.78</v>
+        <v>56.47</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>81.39</v>
+        <v>60.85</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>82.87</v>
+        <v>62.14</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>93.6</v>
+        <v>52.47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4454,16 +4454,16 @@
         <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>87.76</v>
+        <v>57.82</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>81.35</v>
+        <v>64.9</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>82.61</v>
+        <v>70.24</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>93.78</v>
+        <v>49.86</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4474,16 +4474,16 @@
         <v>15</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>88.44</v>
+        <v>73.28</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>81.56</v>
+        <v>70.44</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>80.06</v>
+        <v>65.64</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>99.06</v>
+        <v>83.97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4494,16 +4494,16 @@
         <v>15</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>88.07</v>
+        <v>69.99</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>80.74</v>
+        <v>67.36</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>78.98</v>
+        <v>63.91</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>99.82</v>
+        <v>78.85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,16 +4514,16 @@
         <v>15</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,16 +4534,16 @@
         <v>15</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>87.36</v>
+        <v>52.3</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>80.66</v>
+        <v>58.75</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>82.34</v>
+        <v>60.07</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>93.3</v>
+        <v>46.66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,16 +4554,16 @@
         <v>15</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>87.54</v>
+        <v>52.65</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>81.02</v>
+        <v>62.7</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>82.48</v>
+        <v>69.97</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>93.5</v>
+        <v>43.07</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4574,16 +4574,16 @@
         <v>16</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>88.55</v>
+        <v>62.12</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>81.97</v>
+        <v>64.22</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>81.06</v>
+        <v>64.36</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>97.8</v>
+        <v>61.38</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4594,16 +4594,16 @@
         <v>16</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>88.38</v>
+        <v>63.45</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>81.48</v>
+        <v>63.74</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>80.12</v>
+        <v>62.61</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>98.82</v>
+        <v>65.53</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4614,16 +4614,16 @@
         <v>16</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4634,16 +4634,16 @@
         <v>16</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>87.01</v>
+        <v>57.44</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>80.43</v>
+        <v>60.56</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>83.06</v>
+        <v>60.97</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>91.56</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4654,16 +4654,16 @@
         <v>16</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>86.88</v>
+        <v>53.88</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>80.37</v>
+        <v>61.73</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>83.62</v>
+        <v>66.18</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>90.68</v>
+        <v>46.27</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,7 +4723,7 @@
         <v>3.76</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4774,16 +4774,16 @@
         <v>18</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>88.39</v>
+        <v>72.36</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>81.43</v>
+        <v>69.27</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>79.88</v>
+        <v>64.48</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>99.27</v>
+        <v>83.26</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4794,16 +4794,16 @@
         <v>18</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>88.18</v>
+        <v>69.63</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>80.95</v>
+        <v>67.49</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>79.11</v>
+        <v>64.36</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>99.93</v>
+        <v>77.09</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4814,16 +4814,16 @@
         <v>18</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4834,16 +4834,16 @@
         <v>18</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>87.17</v>
+        <v>53.22</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>80.82</v>
+        <v>59.98</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>83.68</v>
+        <v>62.37</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>91.15</v>
+        <v>47.14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,16 +4854,16 @@
         <v>18</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>87.52</v>
+        <v>51.53</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>81.51</v>
+        <v>62.47</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>84.6</v>
+        <v>70.4</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>90.81</v>
+        <v>41.55</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4874,16 +4874,16 @@
         <v>19</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>88.6</v>
+        <v>71.56</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>81.8</v>
+        <v>69.54</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>80.24</v>
+        <v>65.77</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>99.22</v>
+        <v>79.27</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4894,16 +4894,16 @@
         <v>19</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>88.27</v>
+        <v>69.65</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>81.11</v>
+        <v>67.49</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>79.28</v>
+        <v>64.28</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>99.88</v>
+        <v>77.12</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4914,16 +4914,16 @@
         <v>19</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4934,16 +4934,16 @@
         <v>19</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>87.5</v>
+        <v>56.76</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>81.19</v>
+        <v>61.37</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>83.74</v>
+        <v>62.93</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>91.89</v>
+        <v>52.57</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,16 +4954,16 @@
         <v>19</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>87.66</v>
+        <v>55.06</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>81.23</v>
+        <v>63.67</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>83.12</v>
+        <v>70.19</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>93</v>
+        <v>46.02</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4974,16 +4974,16 @@
         <v>20</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>88.86</v>
+        <v>69.22</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>82.46</v>
+        <v>69.02</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>81.34</v>
+        <v>67.44</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>98.17</v>
+        <v>71.99</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4994,16 +4994,16 @@
         <v>20</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>88.42</v>
+        <v>68.99</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>81.39</v>
+        <v>67.3</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>79.55</v>
+        <v>64.56</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>99.81</v>
+        <v>75.25</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5014,16 +5014,16 @@
         <v>20</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>83.94</v>
+        <v>5.47</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>72.78</v>
+        <v>48.63</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>72.78</v>
+        <v>3.76</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,16 +5034,16 @@
         <v>20</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>87.85</v>
+        <v>60.34</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>81.56</v>
+        <v>62.54</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>83.24</v>
+        <v>62.42</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>93.32</v>
+        <v>59.11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5054,16 +5054,16 @@
         <v>20</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>87.67</v>
+        <v>60.55</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>81.35</v>
+        <v>65.87</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>83.05</v>
+        <v>69.84</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>93.04</v>
+        <v>54.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intermediate Updates for Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -115,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -148,6 +148,13 @@
       <i val="true"/>
       <sz val="10"/>
       <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -195,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,6 +212,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,7 +302,7 @@
   </sheetPr>
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="F111"/>
     </sheetView>
   </sheetViews>
@@ -2989,8 +3004,8 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C103" activeCellId="0" sqref="C103"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4026,403 +4041,427 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="0" t="n">
-        <v>72.64</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>74.76</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>76</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>70.15</v>
+      <c r="C65" s="3" t="n">
+        <v>76.39</v>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>75.55</v>
+      </c>
+      <c r="E65" s="3" t="n">
+        <v>74.46</v>
+      </c>
+      <c r="F65" s="3" t="n">
+        <v>79.01</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="0" t="n">
-        <v>72.86</v>
-      </c>
-      <c r="D66" s="0" t="n">
+      <c r="C66" s="3" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>70.63</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>79.57</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>57.92</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="3" t="n">
+        <v>67.78</v>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>52.15</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>51.91</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>99.28</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="3" t="n">
+        <v>70.08</v>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>69.8</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>69.89</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>70.66</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>71.56</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>75.45</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>68.76</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="3" t="n">
+        <v>73.74</v>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>74.83</v>
+      </c>
+      <c r="E71" s="3" t="n">
+        <v>78.03</v>
+      </c>
+      <c r="F71" s="3" t="n">
         <v>70.74</v>
       </c>
-      <c r="E66" s="0" t="n">
-        <v>65.96</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <v>82.66</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="3" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>71.99</v>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>78.63</v>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" s="0" t="n">
-        <v>10.54</v>
-      </c>
-      <c r="D67" s="0" t="n">
-        <v>53.37</v>
-      </c>
-      <c r="E67" s="0" t="n">
-        <v>77.16</v>
-      </c>
-      <c r="F67" s="0" t="n">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="0" t="n">
-        <v>67.34</v>
-      </c>
-      <c r="D68" s="0" t="n">
+      <c r="B73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="3" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="3" t="n">
+        <v>70.3</v>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>68.46</v>
+      </c>
+      <c r="F74" s="3" t="n">
+        <v>72.63</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>69.51</v>
+      </c>
+      <c r="D75" s="3" t="n">
         <v>71.06</v>
       </c>
-      <c r="E68" s="0" t="n">
-        <v>74.01</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <v>62.15</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="E75" s="3" t="n">
+        <v>74.73</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>65.66</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>73.74</v>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>74.83</v>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>78.03</v>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>70.74</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="3" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>71.99</v>
+      </c>
+      <c r="E78" s="3" t="n">
+        <v>78.63</v>
+      </c>
+      <c r="F78" s="3" t="n">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="3" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="3" t="n">
+        <v>70.3</v>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="E80" s="3" t="n">
+        <v>68.46</v>
+      </c>
+      <c r="F80" s="3" t="n">
+        <v>72.63</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" s="0" t="n">
-        <v>65.44</v>
-      </c>
-      <c r="D69" s="0" t="n">
-        <v>66.46</v>
-      </c>
-      <c r="E69" s="0" t="n">
-        <v>64.46</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <v>66.99</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="B81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>69.51</v>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>71.06</v>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>74.73</v>
+      </c>
+      <c r="F81" s="3" t="n">
+        <v>65.66</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="0" t="n">
-        <v>74.31</v>
-      </c>
-      <c r="D71" s="0" t="n">
-        <v>74.15</v>
-      </c>
-      <c r="E71" s="0" t="n">
-        <v>71.48</v>
-      </c>
-      <c r="F71" s="0" t="n">
-        <v>78.15</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="B83" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="3" t="n">
+        <v>70.69</v>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>73.39</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>81.16</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>63.63</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <v>72.92</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>71.78</v>
-      </c>
-      <c r="E72" s="0" t="n">
-        <v>67.83</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <v>80.17</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="B84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="3" t="n">
+        <v>69.35</v>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>71.81</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>78.73</v>
+      </c>
+      <c r="F84" s="3" t="n">
+        <v>63.28</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" s="0" t="n">
+      <c r="B85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="3" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D85" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="E73" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74" s="0" t="n">
-        <v>68.55</v>
-      </c>
-      <c r="D74" s="0" t="n">
-        <v>71.27</v>
-      </c>
-      <c r="E74" s="0" t="n">
-        <v>72.71</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>65.07</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="E85" s="3" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="F85" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="3" t="n">
+        <v>66.39</v>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>64.52</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="F86" s="3" t="n">
+        <v>69.64</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B75" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" s="0" t="n">
-        <v>67</v>
-      </c>
-      <c r="D75" s="0" t="n">
-        <v>68.54</v>
-      </c>
-      <c r="E75" s="0" t="n">
-        <v>67.82</v>
-      </c>
-      <c r="F75" s="0" t="n">
-        <v>66.52</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C77" s="0" t="n">
-        <v>74.31</v>
-      </c>
-      <c r="D77" s="0" t="n">
-        <v>74.15</v>
-      </c>
-      <c r="E77" s="0" t="n">
-        <v>71.48</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>78.15</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="0" t="n">
-        <v>72.92</v>
-      </c>
-      <c r="D78" s="0" t="n">
-        <v>71.78</v>
-      </c>
-      <c r="E78" s="0" t="n">
-        <v>67.83</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <v>80.17</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D79" s="0" t="n">
-        <v>51.51</v>
-      </c>
-      <c r="E79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" s="0" t="n">
-        <v>68.97</v>
-      </c>
-      <c r="D80" s="0" t="n">
-        <v>71.78</v>
-      </c>
-      <c r="E80" s="0" t="n">
-        <v>73.23</v>
-      </c>
-      <c r="F80" s="0" t="n">
-        <v>65.74</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="0" t="n">
-        <v>68.55</v>
-      </c>
-      <c r="D81" s="0" t="n">
-        <v>71.27</v>
-      </c>
-      <c r="E81" s="0" t="n">
-        <v>72.71</v>
-      </c>
-      <c r="F81" s="0" t="n">
-        <v>65.07</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B83" s="0" t="s">
+      <c r="B87" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="0" t="n">
-        <v>75.41</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>73.79</v>
-      </c>
-      <c r="E83" s="0" t="n">
-        <v>68.32</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>85.03</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>74.07</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="E84" s="0" t="n">
-        <v>68.13</v>
-      </c>
-      <c r="F84" s="0" t="n">
-        <v>82.53</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>51.51</v>
-      </c>
-      <c r="E85" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C86" s="0" t="n">
-        <v>65.23</v>
-      </c>
-      <c r="D86" s="0" t="n">
-        <v>70.41</v>
-      </c>
-      <c r="E86" s="0" t="n">
-        <v>75.62</v>
-      </c>
-      <c r="F86" s="0" t="n">
-        <v>57.79</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C87" s="0" t="n">
-        <v>62.96</v>
-      </c>
-      <c r="D87" s="0" t="n">
-        <v>68.69</v>
-      </c>
-      <c r="E87" s="0" t="n">
-        <v>73.57</v>
-      </c>
-      <c r="F87" s="0" t="n">
-        <v>55.62</v>
+      <c r="C87" s="3" t="n">
+        <v>71.37</v>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>71.2</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>71.29</v>
+      </c>
+      <c r="F87" s="3" t="n">
+        <v>71.77</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,16 +4472,16 @@
         <v>15</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>75.83</v>
+        <v>69.6</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>73.54</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>67.19</v>
+        <v>83.98</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>87.8</v>
+        <v>59.94</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4453,16 +4492,16 @@
         <v>15</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>74.24</v>
+        <v>70.09</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>72.64</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>68.28</v>
+        <v>78.87</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>82.63</v>
+        <v>63.98</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4473,16 +4512,16 @@
         <v>15</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>0</v>
+        <v>67.63</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>51.51</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>0</v>
+        <v>51.51</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4493,16 +4532,16 @@
         <v>15</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>61.61</v>
+        <v>64.19</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>68.58</v>
+        <v>61.45</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>75.07</v>
+        <v>60.46</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>52.59</v>
+        <v>68.91</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4513,516 +4552,540 @@
         <v>15</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>61.04</v>
+        <v>72.11</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>67.79</v>
+        <v>71.42</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>73.8</v>
+        <v>70.84</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>52.57</v>
+        <v>73.68</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C95" s="0" t="n">
+      <c r="C95" s="3" t="n">
         <v>68.9</v>
       </c>
-      <c r="D95" s="0" t="n">
+      <c r="D95" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="E95" s="0" t="n">
+      <c r="E95" s="3" t="n">
         <v>67.14</v>
       </c>
-      <c r="F95" s="0" t="n">
+      <c r="F95" s="3" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C96" s="0" t="n">
+      <c r="C96" s="3" t="n">
         <v>69.32</v>
       </c>
-      <c r="D96" s="0" t="n">
+      <c r="D96" s="3" t="n">
         <v>69.26</v>
       </c>
-      <c r="E96" s="0" t="n">
+      <c r="E96" s="3" t="n">
         <v>67.24</v>
       </c>
-      <c r="F96" s="0" t="n">
+      <c r="F96" s="3" t="n">
         <v>73.46</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="0" t="n">
+      <c r="C97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D97" s="0" t="n">
+      <c r="D97" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="E97" s="0" t="n">
+      <c r="E97" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F97" s="0" t="n">
+      <c r="F97" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B98" s="0" t="s">
+      <c r="A98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C98" s="0" t="n">
+      <c r="C98" s="3" t="n">
         <v>57.61</v>
       </c>
-      <c r="D98" s="0" t="n">
+      <c r="D98" s="3" t="n">
         <v>65.95</v>
       </c>
-      <c r="E98" s="0" t="n">
+      <c r="E98" s="3" t="n">
         <v>71.96</v>
       </c>
-      <c r="F98" s="0" t="n">
+      <c r="F98" s="3" t="n">
         <v>48.49</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C99" s="0" t="n">
+      <c r="C99" s="3" t="n">
         <v>57.9</v>
       </c>
-      <c r="D99" s="0" t="n">
+      <c r="D99" s="3" t="n">
         <v>66.46</v>
       </c>
-      <c r="E99" s="0" t="n">
+      <c r="E99" s="3" t="n">
         <v>73.77</v>
       </c>
-      <c r="F99" s="0" t="n">
+      <c r="F99" s="3" t="n">
         <v>47.99</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C101" s="0" t="n">
+      <c r="C101" s="4" t="n">
         <v>73.48</v>
       </c>
-      <c r="D101" s="0" t="n">
+      <c r="D101" s="4" t="n">
         <v>74.48</v>
       </c>
-      <c r="E101" s="0" t="n">
+      <c r="E101" s="4" t="n">
         <v>77.34</v>
       </c>
-      <c r="F101" s="0" t="n">
+      <c r="F101" s="4" t="n">
         <v>70.6</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C102" s="0" t="n">
+      <c r="C102" s="4" t="n">
         <v>70.18</v>
       </c>
-      <c r="D102" s="0" t="n">
+      <c r="D102" s="4" t="n">
         <v>72.35</v>
       </c>
-      <c r="E102" s="0" t="n">
+      <c r="E102" s="4" t="n">
         <v>78.38</v>
       </c>
-      <c r="F102" s="0" t="n">
+      <c r="F102" s="4" t="n">
         <v>64.32</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C103" s="0" t="n">
+      <c r="C103" s="4" t="n">
         <v>67.63</v>
       </c>
-      <c r="D103" s="0" t="n">
+      <c r="D103" s="4" t="n">
         <v>51.51</v>
       </c>
-      <c r="E103" s="0" t="n">
+      <c r="E103" s="4" t="n">
         <v>51.51</v>
       </c>
-      <c r="F103" s="0" t="n">
+      <c r="F103" s="4" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B104" s="0" t="s">
+      <c r="A104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="0" t="n">
+      <c r="C104" s="4" t="n">
         <v>68.06</v>
       </c>
-      <c r="D104" s="0" t="n">
+      <c r="D104" s="4" t="n">
         <v>66.92</v>
       </c>
-      <c r="E104" s="0" t="n">
+      <c r="E104" s="4" t="n">
         <v>66.86</v>
       </c>
-      <c r="F104" s="0" t="n">
+      <c r="F104" s="4" t="n">
         <v>69.94</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C105" s="0" t="n">
+      <c r="C105" s="4" t="n">
         <v>70.29</v>
       </c>
-      <c r="D105" s="0" t="n">
+      <c r="D105" s="4" t="n">
         <v>71.49</v>
       </c>
-      <c r="E105" s="0" t="n">
+      <c r="E105" s="4" t="n">
         <v>73.57</v>
       </c>
-      <c r="F105" s="0" t="n">
+      <c r="F105" s="4" t="n">
         <v>67.73</v>
       </c>
     </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+    </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="A107" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="B107" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C107" s="0" t="n">
-        <v>75.03</v>
-      </c>
-      <c r="D107" s="0" t="n">
+      <c r="C107" s="4" t="n">
+        <v>68.69</v>
+      </c>
+      <c r="D107" s="4" t="n">
         <v>72.71</v>
       </c>
-      <c r="E107" s="0" t="n">
-        <v>66.75</v>
-      </c>
-      <c r="F107" s="0" t="n">
-        <v>86.7</v>
+      <c r="E107" s="4" t="n">
+        <v>82.81</v>
+      </c>
+      <c r="F107" s="4" t="n">
+        <v>59.5</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C108" s="0" t="n">
-        <v>73.42</v>
-      </c>
-      <c r="D108" s="0" t="n">
+      <c r="C108" s="4" t="n">
+        <v>69.98</v>
+      </c>
+      <c r="D108" s="4" t="n">
         <v>72.21</v>
       </c>
-      <c r="E108" s="0" t="n">
-        <v>67.93</v>
-      </c>
-      <c r="F108" s="0" t="n">
-        <v>81.37</v>
+      <c r="E108" s="4" t="n">
+        <v>78.89</v>
+      </c>
+      <c r="F108" s="4" t="n">
+        <v>64.17</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C109" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D109" s="0" t="n">
+      <c r="C109" s="4" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D109" s="4" t="n">
         <v>51.51</v>
       </c>
-      <c r="E109" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F109" s="0" t="n">
-        <v>0</v>
+      <c r="E109" s="4" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="F109" s="4" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B110" s="0" t="s">
+      <c r="A110" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C110" s="0" t="n">
-        <v>61.43</v>
-      </c>
-      <c r="D110" s="0" t="n">
+      <c r="C110" s="4" t="n">
+        <v>66.78</v>
+      </c>
+      <c r="D110" s="4" t="n">
         <v>64.8</v>
       </c>
-      <c r="E110" s="0" t="n">
-        <v>65.39</v>
-      </c>
-      <c r="F110" s="0" t="n">
-        <v>58.25</v>
+      <c r="E110" s="4" t="n">
+        <v>63.68</v>
+      </c>
+      <c r="F110" s="4" t="n">
+        <v>70.61</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="B111" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C111" s="0" t="n">
-        <v>61.88</v>
-      </c>
-      <c r="D111" s="0" t="n">
-        <v>69.15</v>
-      </c>
-      <c r="E111" s="0" t="n">
-        <v>76.8</v>
-      </c>
-      <c r="F111" s="0" t="n">
-        <v>52.38</v>
-      </c>
+      <c r="C111" s="4" t="n">
+        <v>71.43</v>
+      </c>
+      <c r="D111" s="4" t="n">
+        <v>70.34</v>
+      </c>
+      <c r="E111" s="4" t="n">
+        <v>69.35</v>
+      </c>
+      <c r="F111" s="4" t="n">
+        <v>74.2</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="A113" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B113" s="0" t="s">
+      <c r="B113" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C113" s="0" t="n">
+      <c r="C113" s="4" t="n">
+        <v>70.69</v>
+      </c>
+      <c r="D113" s="4" t="n">
+        <v>73.39</v>
+      </c>
+      <c r="E113" s="4" t="n">
+        <v>81.16</v>
+      </c>
+      <c r="F113" s="4" t="n">
+        <v>63.63</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114" s="4" t="n">
+        <v>69.35</v>
+      </c>
+      <c r="D114" s="4" t="n">
+        <v>71.81</v>
+      </c>
+      <c r="E114" s="4" t="n">
+        <v>78.73</v>
+      </c>
+      <c r="F114" s="4" t="n">
+        <v>63.28</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="4" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D115" s="4" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="E115" s="4" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="F115" s="4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" s="4" t="n">
+        <v>66.39</v>
+      </c>
+      <c r="D116" s="4" t="n">
+        <v>64.52</v>
+      </c>
+      <c r="E116" s="4" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="F116" s="4" t="n">
+        <v>69.64</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" s="4" t="n">
+        <v>71.37</v>
+      </c>
+      <c r="D117" s="4" t="n">
+        <v>71.2</v>
+      </c>
+      <c r="E117" s="4" t="n">
+        <v>71.29</v>
+      </c>
+      <c r="F117" s="4" t="n">
+        <v>71.77</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C119" s="4" t="n">
+        <v>73.74</v>
+      </c>
+      <c r="D119" s="4" t="n">
         <v>74.83</v>
       </c>
-      <c r="D113" s="0" t="n">
-        <v>73.39</v>
-      </c>
-      <c r="E113" s="0" t="n">
-        <v>68.36</v>
-      </c>
-      <c r="F113" s="0" t="n">
-        <v>83.88</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="E119" s="4" t="n">
+        <v>78.03</v>
+      </c>
+      <c r="F119" s="4" t="n">
+        <v>70.74</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B114" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C114" s="0" t="n">
-        <v>73.25</v>
-      </c>
-      <c r="D114" s="0" t="n">
-        <v>71.81</v>
-      </c>
-      <c r="E114" s="0" t="n">
-        <v>67.51</v>
-      </c>
-      <c r="F114" s="0" t="n">
-        <v>81.59</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="B120" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" s="4" t="n">
+        <v>69.63</v>
+      </c>
+      <c r="D120" s="4" t="n">
+        <v>71.99</v>
+      </c>
+      <c r="E120" s="4" t="n">
+        <v>78.63</v>
+      </c>
+      <c r="F120" s="4" t="n">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C115" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D115" s="0" t="n">
+      <c r="B121" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121" s="4" t="n">
+        <v>67.63</v>
+      </c>
+      <c r="D121" s="4" t="n">
         <v>51.51</v>
       </c>
-      <c r="E115" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F115" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C116" s="0" t="n">
-        <v>61.39</v>
-      </c>
-      <c r="D116" s="0" t="n">
-        <v>64.52</v>
-      </c>
-      <c r="E116" s="0" t="n">
-        <v>64.57</v>
-      </c>
-      <c r="F116" s="0" t="n">
-        <v>58.85</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="E121" s="4" t="n">
+        <v>51.51</v>
+      </c>
+      <c r="F121" s="4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" s="4" t="n">
+        <v>70.3</v>
+      </c>
+      <c r="D122" s="4" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="E122" s="4" t="n">
+        <v>68.46</v>
+      </c>
+      <c r="F122" s="4" t="n">
+        <v>72.63</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C117" s="0" t="n">
-        <v>63.44</v>
-      </c>
-      <c r="D117" s="0" t="n">
-        <v>69.05</v>
-      </c>
-      <c r="E117" s="0" t="n">
-        <v>74.02</v>
-      </c>
-      <c r="F117" s="0" t="n">
-        <v>55.86</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B119" s="0" t="s">
+      <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="0" t="n">
-        <v>75.95</v>
-      </c>
-      <c r="D119" s="0" t="n">
-        <v>74.83</v>
-      </c>
-      <c r="E119" s="0" t="n">
-        <v>71.93</v>
-      </c>
-      <c r="F119" s="0" t="n">
-        <v>79.1</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B120" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C120" s="0" t="n">
-        <v>73.37</v>
-      </c>
-      <c r="D120" s="0" t="n">
-        <v>71.99</v>
-      </c>
-      <c r="E120" s="0" t="n">
-        <v>67.56</v>
-      </c>
-      <c r="F120" s="0" t="n">
-        <v>81.59</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B121" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C121" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D121" s="0" t="n">
-        <v>51.51</v>
-      </c>
-      <c r="E121" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F121" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B122" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C122" s="0" t="n">
-        <v>69.14</v>
-      </c>
-      <c r="D122" s="0" t="n">
-        <v>72.06</v>
-      </c>
-      <c r="E122" s="0" t="n">
-        <v>75.07</v>
-      </c>
-      <c r="F122" s="0" t="n">
-        <v>64.86</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B123" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="0" t="n">
-        <v>66.29</v>
-      </c>
-      <c r="D123" s="0" t="n">
-        <v>68.43</v>
-      </c>
-      <c r="E123" s="0" t="n">
-        <v>68.42</v>
-      </c>
-      <c r="F123" s="0" t="n">
-        <v>64.59</v>
+      <c r="C123" s="4" t="n">
+        <v>69.51</v>
+      </c>
+      <c r="D123" s="4" t="n">
+        <v>71.06</v>
+      </c>
+      <c r="E123" s="4" t="n">
+        <v>74.73</v>
+      </c>
+      <c r="F123" s="4" t="n">
+        <v>65.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inverse results for Ubuntu bi-classifier
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -215,11 +215,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,7 +303,7 @@
   <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="F111"/>
+      <selection pane="topLeft" activeCell="F111" activeCellId="1" sqref="A65:F69 F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3005,7 +3005,7 @@
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
+      <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="A65:F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4048,16 +4048,16 @@
         <v>7</v>
       </c>
       <c r="C65" s="3" t="n">
-        <v>76.39</v>
+        <v>75.89</v>
       </c>
       <c r="D65" s="3" t="n">
-        <v>75.55</v>
+        <v>74.76</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>74.46</v>
+        <v>73.43</v>
       </c>
       <c r="F65" s="3" t="n">
-        <v>79.01</v>
+        <v>79.16</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4068,16 +4068,16 @@
         <v>7</v>
       </c>
       <c r="C66" s="3" t="n">
-        <v>66.67</v>
+        <v>67.44</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>70.63</v>
+        <v>70.74</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>79.57</v>
+        <v>78.33</v>
       </c>
       <c r="F66" s="3" t="n">
-        <v>57.92</v>
+        <v>60.09</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4088,16 +4088,16 @@
         <v>7</v>
       </c>
       <c r="C67" s="3" t="n">
-        <v>67.78</v>
+        <v>68.16</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>52.15</v>
+        <v>53.37</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>51.91</v>
+        <v>52.85</v>
       </c>
       <c r="F67" s="3" t="n">
-        <v>99.28</v>
+        <v>98.51</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4108,16 +4108,16 @@
         <v>7</v>
       </c>
       <c r="C68" s="3" t="n">
-        <v>70.08</v>
+        <v>66.42</v>
       </c>
       <c r="D68" s="3" t="n">
-        <v>69.8</v>
+        <v>66.57</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>69.89</v>
+        <v>67.83</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>70.66</v>
+        <v>65.51</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,22 +4131,22 @@
         <v>71.56</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>73</v>
+        <v>72.17</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>75.45</v>
+        <v>74.04</v>
       </c>
       <c r="F69" s="3" t="n">
-        <v>68.76</v>
+        <v>69.76</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
@@ -4156,16 +4156,16 @@
         <v>12</v>
       </c>
       <c r="C71" s="3" t="n">
-        <v>73.74</v>
+        <v>73.16</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>74.83</v>
+        <v>74.15</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>78.03</v>
+        <v>76.91</v>
       </c>
       <c r="F71" s="3" t="n">
-        <v>70.74</v>
+        <v>70.4</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,16 +4176,16 @@
         <v>12</v>
       </c>
       <c r="C72" s="3" t="n">
-        <v>69.63</v>
+        <v>69.72</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>71.99</v>
+        <v>71.78</v>
       </c>
       <c r="E72" s="3" t="n">
-        <v>78.63</v>
+        <v>77.36</v>
       </c>
       <c r="F72" s="3" t="n">
-        <v>63.5</v>
+        <v>64.41</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4216,16 +4216,16 @@
         <v>12</v>
       </c>
       <c r="C74" s="3" t="n">
-        <v>70.3</v>
+        <v>68.92</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>69.3</v>
+        <v>68.61</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>68.46</v>
+        <v>68.45</v>
       </c>
       <c r="F74" s="3" t="n">
-        <v>72.63</v>
+        <v>69.69</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4236,25 +4236,25 @@
         <v>12</v>
       </c>
       <c r="C75" s="3" t="n">
-        <v>69.51</v>
+        <v>71.45</v>
       </c>
       <c r="D75" s="3" t="n">
-        <v>71.06</v>
+        <v>73.04</v>
       </c>
       <c r="E75" s="3" t="n">
-        <v>74.73</v>
+        <v>76.22</v>
       </c>
       <c r="F75" s="3" t="n">
-        <v>65.66</v>
+        <v>67.58</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
@@ -4264,16 +4264,16 @@
         <v>13</v>
       </c>
       <c r="C77" s="3" t="n">
-        <v>73.74</v>
+        <v>73.16</v>
       </c>
       <c r="D77" s="3" t="n">
-        <v>74.83</v>
+        <v>74.15</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>78.03</v>
+        <v>76.91</v>
       </c>
       <c r="F77" s="3" t="n">
-        <v>70.74</v>
+        <v>70.4</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4284,16 +4284,16 @@
         <v>13</v>
       </c>
       <c r="C78" s="3" t="n">
-        <v>69.63</v>
+        <v>69.72</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>71.99</v>
+        <v>71.78</v>
       </c>
       <c r="E78" s="3" t="n">
-        <v>78.63</v>
+        <v>77.36</v>
       </c>
       <c r="F78" s="3" t="n">
-        <v>63.5</v>
+        <v>64.41</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,16 +4324,16 @@
         <v>13</v>
       </c>
       <c r="C80" s="3" t="n">
-        <v>70.3</v>
+        <v>68.92</v>
       </c>
       <c r="D80" s="3" t="n">
-        <v>69.3</v>
+        <v>68.61</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>68.46</v>
+        <v>68.45</v>
       </c>
       <c r="F80" s="3" t="n">
-        <v>72.63</v>
+        <v>69.69</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4344,25 +4344,25 @@
         <v>13</v>
       </c>
       <c r="C81" s="3" t="n">
-        <v>69.51</v>
+        <v>71.45</v>
       </c>
       <c r="D81" s="3" t="n">
-        <v>71.06</v>
+        <v>73.04</v>
       </c>
       <c r="E81" s="3" t="n">
-        <v>74.73</v>
+        <v>76.22</v>
       </c>
       <c r="F81" s="3" t="n">
-        <v>65.66</v>
+        <v>67.58</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
@@ -4372,16 +4372,16 @@
         <v>14</v>
       </c>
       <c r="C83" s="3" t="n">
-        <v>70.69</v>
+        <v>70.83</v>
       </c>
       <c r="D83" s="3" t="n">
-        <v>73.39</v>
+        <v>73.79</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>81.16</v>
+        <v>81.85</v>
       </c>
       <c r="F83" s="3" t="n">
-        <v>63.63</v>
+        <v>63.09</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,16 +4392,16 @@
         <v>14</v>
       </c>
       <c r="C84" s="3" t="n">
-        <v>69.35</v>
+        <v>70.02</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>71.81</v>
+        <v>72.5</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>78.73</v>
+        <v>78.94</v>
       </c>
       <c r="F84" s="3" t="n">
-        <v>63.28</v>
+        <v>63.86</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4432,16 +4432,16 @@
         <v>14</v>
       </c>
       <c r="C86" s="3" t="n">
-        <v>66.39</v>
+        <v>65.72</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>64.52</v>
+        <v>63.91</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>3.77</v>
+        <v>63.43</v>
       </c>
       <c r="F86" s="3" t="n">
-        <v>69.64</v>
+        <v>68.94</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4452,16 +4452,16 @@
         <v>14</v>
       </c>
       <c r="C87" s="3" t="n">
-        <v>71.37</v>
+        <v>71.28</v>
       </c>
       <c r="D87" s="3" t="n">
-        <v>71.2</v>
+        <v>71.02</v>
       </c>
       <c r="E87" s="3" t="n">
-        <v>71.29</v>
+        <v>71.39</v>
       </c>
       <c r="F87" s="3" t="n">
-        <v>71.77</v>
+        <v>71.84</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4572,16 +4572,16 @@
         <v>16</v>
       </c>
       <c r="C95" s="3" t="n">
-        <v>68.9</v>
+        <v>68.85</v>
       </c>
       <c r="D95" s="3" t="n">
         <v>69.3</v>
       </c>
       <c r="E95" s="3" t="n">
-        <v>67.14</v>
+        <v>71.8</v>
       </c>
       <c r="F95" s="3" t="n">
-        <v>72</v>
+        <v>67.11</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4592,16 +4592,16 @@
         <v>16</v>
       </c>
       <c r="C96" s="3" t="n">
-        <v>69.32</v>
+        <v>68.45</v>
       </c>
       <c r="D96" s="3" t="n">
         <v>69.26</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>67.24</v>
+        <v>72.61</v>
       </c>
       <c r="F96" s="3" t="n">
-        <v>73.46</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4612,16 +4612,16 @@
         <v>16</v>
       </c>
       <c r="C97" s="3" t="n">
-        <v>0</v>
+        <v>67.63</v>
       </c>
       <c r="D97" s="3" t="n">
         <v>51.51</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0</v>
+        <v>51.51</v>
       </c>
       <c r="F97" s="3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4632,16 +4632,16 @@
         <v>16</v>
       </c>
       <c r="C98" s="3" t="n">
-        <v>57.61</v>
+        <v>67.4</v>
       </c>
       <c r="D98" s="3" t="n">
-        <v>65.95</v>
+        <v>64.95</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>71.96</v>
+        <v>63.59</v>
       </c>
       <c r="F98" s="3" t="n">
-        <v>48.49</v>
+        <v>72.32</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4652,439 +4652,439 @@
         <v>16</v>
       </c>
       <c r="C99" s="3" t="n">
-        <v>57.9</v>
+        <v>71.01</v>
       </c>
       <c r="D99" s="3" t="n">
-        <v>66.46</v>
+        <v>68.22</v>
       </c>
       <c r="E99" s="3" t="n">
-        <v>73.77</v>
+        <v>65.94</v>
       </c>
       <c r="F99" s="3" t="n">
-        <v>47.99</v>
+        <v>77.47</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C101" s="4" t="n">
+      <c r="C101" s="3" t="n">
         <v>73.48</v>
       </c>
-      <c r="D101" s="4" t="n">
+      <c r="D101" s="3" t="n">
         <v>74.48</v>
       </c>
-      <c r="E101" s="4" t="n">
+      <c r="E101" s="3" t="n">
         <v>77.34</v>
       </c>
-      <c r="F101" s="4" t="n">
+      <c r="F101" s="3" t="n">
         <v>70.6</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C102" s="4" t="n">
+      <c r="C102" s="3" t="n">
         <v>70.18</v>
       </c>
-      <c r="D102" s="4" t="n">
+      <c r="D102" s="3" t="n">
         <v>72.35</v>
       </c>
-      <c r="E102" s="4" t="n">
+      <c r="E102" s="3" t="n">
         <v>78.38</v>
       </c>
-      <c r="F102" s="4" t="n">
+      <c r="F102" s="3" t="n">
         <v>64.32</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C103" s="4" t="n">
+      <c r="C103" s="3" t="n">
         <v>67.63</v>
       </c>
-      <c r="D103" s="4" t="n">
+      <c r="D103" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="E103" s="4" t="n">
+      <c r="E103" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="F103" s="4" t="n">
+      <c r="F103" s="3" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B104" s="4" t="s">
+      <c r="A104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="4" t="n">
+      <c r="C104" s="3" t="n">
         <v>68.06</v>
       </c>
-      <c r="D104" s="4" t="n">
+      <c r="D104" s="3" t="n">
         <v>66.92</v>
       </c>
-      <c r="E104" s="4" t="n">
+      <c r="E104" s="3" t="n">
         <v>66.86</v>
       </c>
-      <c r="F104" s="4" t="n">
+      <c r="F104" s="3" t="n">
         <v>69.94</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C105" s="4" t="n">
+      <c r="C105" s="3" t="n">
         <v>70.29</v>
       </c>
-      <c r="D105" s="4" t="n">
+      <c r="D105" s="3" t="n">
         <v>71.49</v>
       </c>
-      <c r="E105" s="4" t="n">
+      <c r="E105" s="3" t="n">
         <v>73.57</v>
       </c>
-      <c r="F105" s="4" t="n">
+      <c r="F105" s="3" t="n">
         <v>67.73</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C107" s="4" t="n">
+      <c r="C107" s="3" t="n">
         <v>68.69</v>
       </c>
-      <c r="D107" s="4" t="n">
+      <c r="D107" s="3" t="n">
         <v>72.71</v>
       </c>
-      <c r="E107" s="4" t="n">
+      <c r="E107" s="3" t="n">
         <v>82.81</v>
       </c>
-      <c r="F107" s="4" t="n">
+      <c r="F107" s="3" t="n">
         <v>59.5</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C108" s="4" t="n">
+      <c r="C108" s="3" t="n">
         <v>69.98</v>
       </c>
-      <c r="D108" s="4" t="n">
+      <c r="D108" s="3" t="n">
         <v>72.21</v>
       </c>
-      <c r="E108" s="4" t="n">
+      <c r="E108" s="3" t="n">
         <v>78.89</v>
       </c>
-      <c r="F108" s="4" t="n">
+      <c r="F108" s="3" t="n">
         <v>64.17</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C109" s="4" t="n">
+      <c r="C109" s="3" t="n">
         <v>67.63</v>
       </c>
-      <c r="D109" s="4" t="n">
+      <c r="D109" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="E109" s="4" t="n">
+      <c r="E109" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="F109" s="4" t="n">
+      <c r="F109" s="3" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B110" s="4" t="s">
+      <c r="A110" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C110" s="4" t="n">
+      <c r="C110" s="3" t="n">
         <v>66.78</v>
       </c>
-      <c r="D110" s="4" t="n">
+      <c r="D110" s="3" t="n">
         <v>64.8</v>
       </c>
-      <c r="E110" s="4" t="n">
+      <c r="E110" s="3" t="n">
         <v>63.68</v>
       </c>
-      <c r="F110" s="4" t="n">
+      <c r="F110" s="3" t="n">
         <v>70.61</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C111" s="4" t="n">
+      <c r="C111" s="3" t="n">
         <v>71.43</v>
       </c>
-      <c r="D111" s="4" t="n">
+      <c r="D111" s="3" t="n">
         <v>70.34</v>
       </c>
-      <c r="E111" s="4" t="n">
+      <c r="E111" s="3" t="n">
         <v>69.35</v>
       </c>
-      <c r="F111" s="4" t="n">
+      <c r="F111" s="3" t="n">
         <v>74.2</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C113" s="4" t="n">
+      <c r="C113" s="3" t="n">
         <v>70.69</v>
       </c>
-      <c r="D113" s="4" t="n">
+      <c r="D113" s="3" t="n">
         <v>73.39</v>
       </c>
-      <c r="E113" s="4" t="n">
+      <c r="E113" s="3" t="n">
         <v>81.16</v>
       </c>
-      <c r="F113" s="4" t="n">
+      <c r="F113" s="3" t="n">
         <v>63.63</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C114" s="4" t="n">
+      <c r="C114" s="3" t="n">
         <v>69.35</v>
       </c>
-      <c r="D114" s="4" t="n">
+      <c r="D114" s="3" t="n">
         <v>71.81</v>
       </c>
-      <c r="E114" s="4" t="n">
+      <c r="E114" s="3" t="n">
         <v>78.73</v>
       </c>
-      <c r="F114" s="4" t="n">
+      <c r="F114" s="3" t="n">
         <v>63.28</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C115" s="4" t="n">
+      <c r="C115" s="3" t="n">
         <v>67.63</v>
       </c>
-      <c r="D115" s="4" t="n">
+      <c r="D115" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="E115" s="4" t="n">
+      <c r="E115" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="F115" s="4" t="n">
+      <c r="F115" s="3" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116" s="4" t="s">
+      <c r="A116" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C116" s="4" t="n">
+      <c r="C116" s="3" t="n">
         <v>66.39</v>
       </c>
-      <c r="D116" s="4" t="n">
+      <c r="D116" s="3" t="n">
         <v>64.52</v>
       </c>
-      <c r="E116" s="4" t="n">
+      <c r="E116" s="3" t="n">
         <v>3.77</v>
       </c>
-      <c r="F116" s="4" t="n">
+      <c r="F116" s="3" t="n">
         <v>69.64</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C117" s="4" t="n">
+      <c r="C117" s="3" t="n">
         <v>71.37</v>
       </c>
-      <c r="D117" s="4" t="n">
+      <c r="D117" s="3" t="n">
         <v>71.2</v>
       </c>
-      <c r="E117" s="4" t="n">
+      <c r="E117" s="3" t="n">
         <v>71.29</v>
       </c>
-      <c r="F117" s="4" t="n">
+      <c r="F117" s="3" t="n">
         <v>71.77</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="4"/>
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="4" t="n">
+      <c r="C119" s="3" t="n">
         <v>73.74</v>
       </c>
-      <c r="D119" s="4" t="n">
+      <c r="D119" s="3" t="n">
         <v>74.83</v>
       </c>
-      <c r="E119" s="4" t="n">
+      <c r="E119" s="3" t="n">
         <v>78.03</v>
       </c>
-      <c r="F119" s="4" t="n">
+      <c r="F119" s="3" t="n">
         <v>70.74</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="4" t="n">
+      <c r="C120" s="3" t="n">
         <v>69.63</v>
       </c>
-      <c r="D120" s="4" t="n">
+      <c r="D120" s="3" t="n">
         <v>71.99</v>
       </c>
-      <c r="E120" s="4" t="n">
+      <c r="E120" s="3" t="n">
         <v>78.63</v>
       </c>
-      <c r="F120" s="4" t="n">
+      <c r="F120" s="3" t="n">
         <v>63.5</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="4" t="n">
+      <c r="C121" s="3" t="n">
         <v>67.63</v>
       </c>
-      <c r="D121" s="4" t="n">
+      <c r="D121" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="E121" s="4" t="n">
+      <c r="E121" s="3" t="n">
         <v>51.51</v>
       </c>
-      <c r="F121" s="4" t="n">
+      <c r="F121" s="3" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B122" s="4" t="s">
+      <c r="A122" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C122" s="4" t="n">
+      <c r="C122" s="3" t="n">
         <v>70.3</v>
       </c>
-      <c r="D122" s="4" t="n">
+      <c r="D122" s="3" t="n">
         <v>69.3</v>
       </c>
-      <c r="E122" s="4" t="n">
+      <c r="E122" s="3" t="n">
         <v>68.46</v>
       </c>
-      <c r="F122" s="4" t="n">
+      <c r="F122" s="3" t="n">
         <v>72.63</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="4" t="n">
+      <c r="C123" s="3" t="n">
         <v>69.51</v>
       </c>
-      <c r="D123" s="4" t="n">
+      <c r="D123" s="3" t="n">
         <v>71.06</v>
       </c>
-      <c r="E123" s="4" t="n">
+      <c r="E123" s="3" t="n">
         <v>74.73</v>
       </c>
-      <c r="F123" s="4" t="n">
+      <c r="F123" s="3" t="n">
         <v>65.66</v>
       </c>
     </row>
@@ -5106,8 +5106,8 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B110" activeCellId="1" sqref="A65:F69 B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6743,102 +6743,102 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C101" s="0" t="n">
+      <c r="C101" s="4" t="n">
         <v>68.71</v>
       </c>
-      <c r="D101" s="0" t="n">
+      <c r="D101" s="4" t="n">
         <v>69.41</v>
       </c>
-      <c r="E101" s="0" t="n">
+      <c r="E101" s="4" t="n">
         <v>71.85</v>
       </c>
-      <c r="F101" s="0" t="n">
+      <c r="F101" s="4" t="n">
         <v>66.59</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C102" s="0" t="n">
+      <c r="C102" s="4" t="n">
         <v>65.58</v>
       </c>
-      <c r="D102" s="0" t="n">
+      <c r="D102" s="4" t="n">
         <v>67.56</v>
       </c>
-      <c r="E102" s="0" t="n">
+      <c r="E102" s="4" t="n">
         <v>71.86</v>
       </c>
-      <c r="F102" s="0" t="n">
+      <c r="F102" s="4" t="n">
         <v>61.49</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C103" s="0" t="n">
+      <c r="C103" s="4" t="n">
         <v>59.74</v>
       </c>
-      <c r="D103" s="0" t="n">
+      <c r="D103" s="4" t="n">
         <v>48.63</v>
       </c>
-      <c r="E103" s="0" t="n">
+      <c r="E103" s="4" t="n">
         <v>44.87</v>
       </c>
-      <c r="F103" s="0" t="n">
+      <c r="F103" s="4" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B104" s="0" t="s">
+      <c r="A104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="0" t="n">
+      <c r="C104" s="4" t="n">
         <v>65.05</v>
       </c>
-      <c r="D104" s="0" t="n">
+      <c r="D104" s="4" t="n">
         <v>63.18</v>
       </c>
-      <c r="E104" s="0" t="n">
+      <c r="E104" s="4" t="n">
         <v>63.29</v>
       </c>
-      <c r="F104" s="0" t="n">
+      <c r="F104" s="4" t="n">
         <v>67.55</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C105" s="0" t="n">
+      <c r="C105" s="4" t="n">
         <v>67.13</v>
       </c>
-      <c r="D105" s="0" t="n">
+      <c r="D105" s="4" t="n">
         <v>67.43</v>
       </c>
-      <c r="E105" s="0" t="n">
+      <c r="E105" s="4" t="n">
         <v>69.09</v>
       </c>
-      <c r="F105" s="0" t="n">
+      <c r="F105" s="4" t="n">
         <v>66.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added inverse results for Thunderbird bi-classifier
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -303,7 +303,7 @@
   <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F111" activeCellId="1" sqref="A65:F69 F111"/>
+      <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="A107:F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3004,8 +3004,8 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="A65:F69"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C119" activeCellId="1" sqref="A107:F111 C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5106,8 +5106,8 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B110" activeCellId="1" sqref="A65:F69 B110"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="A107:F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6143,1003 +6143,1059 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="0" t="n">
-        <v>67.6</v>
-      </c>
-      <c r="D65" s="0" t="n">
+      <c r="C65" s="3" t="n">
+        <v>71.61</v>
+      </c>
+      <c r="D65" s="3" t="n">
         <v>69.96</v>
       </c>
-      <c r="E65" s="0" t="n">
-        <v>71.33</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>64.78</v>
+      <c r="E65" s="3" t="n">
+        <v>68.81</v>
+      </c>
+      <c r="F65" s="3" t="n">
+        <v>75.17</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="0" t="n">
-        <v>69.78</v>
-      </c>
-      <c r="D66" s="0" t="n">
+      <c r="C66" s="3" t="n">
+        <v>60.49</v>
+      </c>
+      <c r="D66" s="3" t="n">
         <v>66.07</v>
       </c>
-      <c r="E66" s="0" t="n">
-        <v>61.68</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <v>81.58</v>
+      <c r="E66" s="3" t="n">
+        <v>75.04</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>51.6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>19.09</v>
-      </c>
-      <c r="D67" s="0" t="n">
+      <c r="C67" s="3" t="n">
+        <v>68.38</v>
+      </c>
+      <c r="D67" s="3" t="n">
         <v>54.7</v>
       </c>
-      <c r="E67" s="0" t="n">
-        <v>75.33</v>
-      </c>
-      <c r="F67" s="0" t="n">
-        <v>11.21</v>
+      <c r="E67" s="3" t="n">
+        <v>53.22</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>96.74</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="0" t="s">
+      <c r="A68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="0" t="n">
-        <v>62.35</v>
-      </c>
-      <c r="D68" s="0" t="n">
+      <c r="C68" s="3" t="n">
+        <v>66.55</v>
+      </c>
+      <c r="D68" s="3" t="n">
         <v>64.84</v>
       </c>
-      <c r="E68" s="0" t="n">
-        <v>65.17</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <v>60.4</v>
+      <c r="E68" s="3" t="n">
+        <v>64.57</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>69.24</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="0" t="n">
-        <v>58.54</v>
-      </c>
-      <c r="D69" s="0" t="n">
-        <v>64.64</v>
-      </c>
-      <c r="E69" s="0" t="n">
-        <v>68.92</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <v>51.89</v>
+      <c r="C69" s="3" t="n">
+        <v>65.79</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>65.45</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>66.59</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>65.99</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="0" t="n">
-        <v>68.18</v>
-      </c>
-      <c r="D71" s="0" t="n">
+      <c r="C71" s="3" t="n">
+        <v>68.49</v>
+      </c>
+      <c r="D71" s="3" t="n">
         <v>68.59</v>
       </c>
-      <c r="E71" s="0" t="n">
-        <v>67.47</v>
-      </c>
-      <c r="F71" s="0" t="n">
-        <v>70.03</v>
+      <c r="E71" s="3" t="n">
+        <v>70.32</v>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>67.7</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C72" s="0" t="n">
-        <v>68.31</v>
-      </c>
-      <c r="D72" s="0" t="n">
+      <c r="C72" s="3" t="n">
+        <v>64.58</v>
+      </c>
+      <c r="D72" s="3" t="n">
         <v>66.75</v>
       </c>
-      <c r="E72" s="0" t="n">
+      <c r="E72" s="3" t="n">
+        <v>71.17</v>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>60.33</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>48.63</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="3" t="n">
+        <v>63.88</v>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>62.76</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>63.29</v>
+      </c>
+      <c r="F74" s="3" t="n">
+        <v>65.23</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>64.9</v>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>66.07</v>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>68.93</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>62.15</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>68.49</v>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>68.59</v>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>70.32</v>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="3" t="n">
+        <v>64.58</v>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>66.75</v>
+      </c>
+      <c r="E78" s="3" t="n">
+        <v>71.17</v>
+      </c>
+      <c r="F78" s="3" t="n">
+        <v>60.33</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>48.63</v>
+      </c>
+      <c r="E79" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="3" t="n">
+        <v>63.88</v>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>62.76</v>
+      </c>
+      <c r="E80" s="3" t="n">
+        <v>63.29</v>
+      </c>
+      <c r="F80" s="3" t="n">
+        <v>65.23</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>64.9</v>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>66.07</v>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>68.93</v>
+      </c>
+      <c r="F81" s="3" t="n">
+        <v>62.15</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="3" t="n">
+        <v>67.83</v>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>70.35</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>76.03</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>62.04</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="3" t="n">
+        <v>63.97</v>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>67.52</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>73.99</v>
+      </c>
+      <c r="F84" s="3" t="n">
+        <v>57.37</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>48.63</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F85" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="3" t="n">
+        <v>64.27</v>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>60.92</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>60.41</v>
+      </c>
+      <c r="F86" s="3" t="n">
+        <v>69.51</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="3" t="n">
+        <v>68.66</v>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>67.72</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>68.02</v>
+      </c>
+      <c r="F87" s="3" t="n">
+        <v>70.06</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="3" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>70.44</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>78.96</v>
+      </c>
+      <c r="F89" s="3" t="n">
+        <v>58.18</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="3" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>67.36</v>
+      </c>
+      <c r="E90" s="3" t="n">
+        <v>73.88</v>
+      </c>
+      <c r="F90" s="3" t="n">
+        <v>57.48</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>48.63</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F91" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="3" t="n">
+        <v>63.31</v>
+      </c>
+      <c r="D92" s="3" t="n">
+        <v>58.81</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>57.89</v>
+      </c>
+      <c r="F92" s="3" t="n">
+        <v>70.34</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="3" t="n">
+        <v>67.43</v>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>65.39</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>65.16</v>
+      </c>
+      <c r="F93" s="3" t="n">
+        <v>70.94</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="3" t="n">
+        <v>65.7</v>
+      </c>
+      <c r="D95" s="3" t="n">
         <v>64.22</v>
       </c>
-      <c r="F72" s="0" t="n">
-        <v>74.4</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="E95" s="3" t="n">
+        <v>64.93</v>
+      </c>
+      <c r="F95" s="3" t="n">
+        <v>67.79</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="3" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="D96" s="3" t="n">
+        <v>63.74</v>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>65.66</v>
+      </c>
+      <c r="F96" s="3" t="n">
+        <v>62.74</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D73" s="0" t="n">
+      <c r="B97" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D97" s="3" t="n">
         <v>48.63</v>
       </c>
-      <c r="E73" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74" s="0" t="n">
-        <v>61.15</v>
-      </c>
-      <c r="D74" s="0" t="n">
-        <v>62.73</v>
-      </c>
-      <c r="E74" s="0" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>60.57</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="E97" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F97" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="3" t="n">
+        <v>62.98</v>
+      </c>
+      <c r="D98" s="3" t="n">
+        <v>60.63</v>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>60.98</v>
+      </c>
+      <c r="F98" s="3" t="n">
+        <v>66.21</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B75" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" s="0" t="n">
-        <v>61.97</v>
-      </c>
-      <c r="D75" s="0" t="n">
-        <v>65.71</v>
-      </c>
-      <c r="E75" s="0" t="n">
-        <v>68.02</v>
-      </c>
-      <c r="F75" s="0" t="n">
-        <v>57.73</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="B99" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="3" t="n">
+        <v>65.79</v>
+      </c>
+      <c r="D99" s="3" t="n">
+        <v>63.19</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>62.81</v>
+      </c>
+      <c r="F99" s="3" t="n">
+        <v>70.05</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C77" s="0" t="n">
-        <v>68.18</v>
-      </c>
-      <c r="D77" s="0" t="n">
-        <v>68.59</v>
-      </c>
-      <c r="E77" s="0" t="n">
-        <v>67.47</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>70.03</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="B101" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101" s="3" t="n">
+        <v>68.71</v>
+      </c>
+      <c r="D101" s="3" t="n">
+        <v>69.41</v>
+      </c>
+      <c r="E101" s="3" t="n">
+        <v>71.85</v>
+      </c>
+      <c r="F101" s="3" t="n">
+        <v>66.59</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="0" t="n">
-        <v>68.31</v>
-      </c>
-      <c r="D78" s="0" t="n">
-        <v>66.75</v>
-      </c>
-      <c r="E78" s="0" t="n">
-        <v>64.22</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <v>74.4</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="B102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" s="3" t="n">
+        <v>65.58</v>
+      </c>
+      <c r="D102" s="3" t="n">
+        <v>67.56</v>
+      </c>
+      <c r="E102" s="3" t="n">
+        <v>71.86</v>
+      </c>
+      <c r="F102" s="3" t="n">
+        <v>61.49</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D79" s="0" t="n">
+      <c r="B103" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D103" s="3" t="n">
         <v>48.63</v>
       </c>
-      <c r="E79" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" s="0" t="n">
-        <v>61.15</v>
-      </c>
-      <c r="D80" s="0" t="n">
-        <v>62.73</v>
-      </c>
-      <c r="E80" s="0" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="F80" s="0" t="n">
-        <v>60.57</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="E103" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F103" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="3" t="n">
+        <v>65.05</v>
+      </c>
+      <c r="D104" s="3" t="n">
+        <v>63.18</v>
+      </c>
+      <c r="E104" s="3" t="n">
+        <v>63.29</v>
+      </c>
+      <c r="F104" s="3" t="n">
+        <v>67.55</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B81" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="0" t="n">
-        <v>61.97</v>
-      </c>
-      <c r="D81" s="0" t="n">
-        <v>65.71</v>
-      </c>
-      <c r="E81" s="0" t="n">
-        <v>68.02</v>
-      </c>
-      <c r="F81" s="0" t="n">
-        <v>57.73</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="B105" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" s="3" t="n">
+        <v>67.13</v>
+      </c>
+      <c r="D105" s="3" t="n">
+        <v>67.43</v>
+      </c>
+      <c r="E105" s="3" t="n">
+        <v>69.09</v>
+      </c>
+      <c r="F105" s="3" t="n">
+        <v>66.06</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C83" s="0" t="n">
-        <v>72.15</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>70.35</v>
-      </c>
-      <c r="E83" s="0" t="n">
-        <v>66.66</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>79.11</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="B107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="D107" s="3" t="n">
+        <v>69.27</v>
+      </c>
+      <c r="E107" s="3" t="n">
+        <v>77.55</v>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>56.39</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>70.19</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>67.52</v>
-      </c>
-      <c r="E84" s="0" t="n">
-        <v>63.94</v>
-      </c>
-      <c r="F84" s="0" t="n">
-        <v>79.19</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="B108" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="3" t="n">
+        <v>64.76</v>
+      </c>
+      <c r="D108" s="3" t="n">
+        <v>67.49</v>
+      </c>
+      <c r="E108" s="3" t="n">
+        <v>72.74</v>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>59.27</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B85" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D85" s="0" t="n">
+      <c r="B109" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C109" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D109" s="3" t="n">
         <v>48.63</v>
       </c>
-      <c r="E85" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C86" s="0" t="n">
-        <v>56.47</v>
-      </c>
-      <c r="D86" s="0" t="n">
+      <c r="E109" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F109" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" s="3" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="D110" s="3" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="E110" s="3" t="n">
+        <v>58.97</v>
+      </c>
+      <c r="F110" s="3" t="n">
+        <v>72.82</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C111" s="3" t="n">
+        <v>68.14</v>
+      </c>
+      <c r="D111" s="3" t="n">
+        <v>65.55</v>
+      </c>
+      <c r="E111" s="3" t="n">
+        <v>64.6</v>
+      </c>
+      <c r="F111" s="3" t="n">
+        <v>72.98</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" s="3" t="n">
+        <v>66.91</v>
+      </c>
+      <c r="D113" s="3" t="n">
+        <v>69.54</v>
+      </c>
+      <c r="E113" s="3" t="n">
+        <v>75.05</v>
+      </c>
+      <c r="F113" s="3" t="n">
         <v>60.85</v>
       </c>
-      <c r="E86" s="0" t="n">
-        <v>62.14</v>
-      </c>
-      <c r="F86" s="0" t="n">
-        <v>52.47</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114" s="3" t="n">
+        <v>64.69</v>
+      </c>
+      <c r="D114" s="3" t="n">
+        <v>67.49</v>
+      </c>
+      <c r="E114" s="3" t="n">
+        <v>72.66</v>
+      </c>
+      <c r="F114" s="3" t="n">
+        <v>59.09</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D115" s="3" t="n">
+        <v>48.63</v>
+      </c>
+      <c r="E115" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F115" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" s="3" t="n">
+        <v>64.87</v>
+      </c>
+      <c r="D116" s="3" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="E116" s="3" t="n">
+        <v>60.8</v>
+      </c>
+      <c r="F116" s="3" t="n">
+        <v>70.51</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C87" s="0" t="n">
-        <v>57.82</v>
-      </c>
-      <c r="D87" s="0" t="n">
-        <v>64.9</v>
-      </c>
-      <c r="E87" s="0" t="n">
-        <v>70.24</v>
-      </c>
-      <c r="F87" s="0" t="n">
-        <v>49.86</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="B117" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" s="3" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="D117" s="3" t="n">
+        <v>66.33</v>
+      </c>
+      <c r="E117" s="3" t="n">
+        <v>66.13</v>
+      </c>
+      <c r="F117" s="3" t="n">
+        <v>69.64</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C89" s="0" t="n">
-        <v>73.28</v>
-      </c>
-      <c r="D89" s="0" t="n">
-        <v>70.44</v>
-      </c>
-      <c r="E89" s="0" t="n">
-        <v>65.64</v>
-      </c>
-      <c r="F89" s="0" t="n">
-        <v>83.97</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="B119" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C119" s="3" t="n">
+        <v>68.61</v>
+      </c>
+      <c r="D119" s="3" t="n">
+        <v>69.05</v>
+      </c>
+      <c r="E119" s="3" t="n">
+        <v>71.11</v>
+      </c>
+      <c r="F119" s="3" t="n">
+        <v>66.97</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="0" t="n">
-        <v>69.99</v>
-      </c>
-      <c r="D90" s="0" t="n">
-        <v>67.36</v>
-      </c>
-      <c r="E90" s="0" t="n">
-        <v>63.91</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>78.85</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="B120" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" s="3" t="n">
+        <v>65.08</v>
+      </c>
+      <c r="D120" s="3" t="n">
+        <v>67.27</v>
+      </c>
+      <c r="E120" s="3" t="n">
+        <v>71.67</v>
+      </c>
+      <c r="F120" s="3" t="n">
+        <v>60.52</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C91" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D91" s="0" t="n">
-        <v>48.63</v>
-      </c>
-      <c r="E91" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F91" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>52.3</v>
-      </c>
-      <c r="D92" s="0" t="n">
-        <v>58.75</v>
-      </c>
-      <c r="E92" s="0" t="n">
-        <v>60.07</v>
-      </c>
-      <c r="F92" s="0" t="n">
-        <v>46.66</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="B121" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121" s="3" t="n">
+        <v>59.74</v>
+      </c>
+      <c r="D121" s="3" t="n">
+        <v>48.69</v>
+      </c>
+      <c r="E121" s="3" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="F121" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" s="3" t="n">
+        <v>64.52</v>
+      </c>
+      <c r="D122" s="3" t="n">
+        <v>62.89</v>
+      </c>
+      <c r="E122" s="3" t="n">
+        <v>62.94</v>
+      </c>
+      <c r="F122" s="3" t="n">
+        <v>66.77</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B93" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C93" s="0" t="n">
-        <v>52.65</v>
-      </c>
-      <c r="D93" s="0" t="n">
-        <v>62.7</v>
-      </c>
-      <c r="E93" s="0" t="n">
-        <v>69.97</v>
-      </c>
-      <c r="F93" s="0" t="n">
-        <v>43.07</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C95" s="0" t="n">
-        <v>62.12</v>
-      </c>
-      <c r="D95" s="0" t="n">
-        <v>64.22</v>
-      </c>
-      <c r="E95" s="0" t="n">
-        <v>64.36</v>
-      </c>
-      <c r="F95" s="0" t="n">
-        <v>61.38</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B96" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C96" s="0" t="n">
-        <v>63.45</v>
-      </c>
-      <c r="D96" s="0" t="n">
-        <v>63.74</v>
-      </c>
-      <c r="E96" s="0" t="n">
-        <v>62.61</v>
-      </c>
-      <c r="F96" s="0" t="n">
-        <v>65.53</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C97" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D97" s="0" t="n">
-        <v>48.63</v>
-      </c>
-      <c r="E97" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F97" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B98" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C98" s="0" t="n">
-        <v>57.44</v>
-      </c>
-      <c r="D98" s="0" t="n">
-        <v>60.56</v>
-      </c>
-      <c r="E98" s="0" t="n">
-        <v>60.97</v>
-      </c>
-      <c r="F98" s="0" t="n">
-        <v>55.4</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C99" s="0" t="n">
-        <v>53.88</v>
-      </c>
-      <c r="D99" s="0" t="n">
-        <v>61.73</v>
-      </c>
-      <c r="E99" s="0" t="n">
-        <v>66.18</v>
-      </c>
-      <c r="F99" s="0" t="n">
-        <v>46.27</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C101" s="4" t="n">
-        <v>68.71</v>
-      </c>
-      <c r="D101" s="4" t="n">
-        <v>69.41</v>
-      </c>
-      <c r="E101" s="4" t="n">
-        <v>71.85</v>
-      </c>
-      <c r="F101" s="4" t="n">
-        <v>66.59</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C102" s="4" t="n">
-        <v>65.58</v>
-      </c>
-      <c r="D102" s="4" t="n">
-        <v>67.56</v>
-      </c>
-      <c r="E102" s="4" t="n">
-        <v>71.86</v>
-      </c>
-      <c r="F102" s="4" t="n">
-        <v>61.49</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C103" s="4" t="n">
-        <v>59.74</v>
-      </c>
-      <c r="D103" s="4" t="n">
-        <v>48.63</v>
-      </c>
-      <c r="E103" s="4" t="n">
-        <v>44.87</v>
-      </c>
-      <c r="F103" s="4" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C104" s="4" t="n">
-        <v>65.05</v>
-      </c>
-      <c r="D104" s="4" t="n">
-        <v>63.18</v>
-      </c>
-      <c r="E104" s="4" t="n">
-        <v>63.29</v>
-      </c>
-      <c r="F104" s="4" t="n">
-        <v>67.55</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C105" s="4" t="n">
-        <v>67.13</v>
-      </c>
-      <c r="D105" s="4" t="n">
+      <c r="B123" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C123" s="3" t="n">
+        <v>66.85</v>
+      </c>
+      <c r="D123" s="3" t="n">
         <v>67.43</v>
       </c>
-      <c r="E105" s="4" t="n">
-        <v>69.09</v>
-      </c>
-      <c r="F105" s="4" t="n">
-        <v>66.06</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B107" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C107" s="0" t="n">
-        <v>72.36</v>
-      </c>
-      <c r="D107" s="0" t="n">
-        <v>69.27</v>
-      </c>
-      <c r="E107" s="0" t="n">
-        <v>64.48</v>
-      </c>
-      <c r="F107" s="0" t="n">
-        <v>83.26</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B108" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C108" s="0" t="n">
-        <v>69.63</v>
-      </c>
-      <c r="D108" s="0" t="n">
-        <v>67.49</v>
-      </c>
-      <c r="E108" s="0" t="n">
-        <v>64.36</v>
-      </c>
-      <c r="F108" s="0" t="n">
-        <v>77.09</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C109" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D109" s="0" t="n">
-        <v>48.63</v>
-      </c>
-      <c r="E109" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F109" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B110" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C110" s="0" t="n">
-        <v>53.22</v>
-      </c>
-      <c r="D110" s="0" t="n">
-        <v>59.98</v>
-      </c>
-      <c r="E110" s="0" t="n">
-        <v>62.37</v>
-      </c>
-      <c r="F110" s="0" t="n">
-        <v>47.14</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B111" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C111" s="0" t="n">
-        <v>51.53</v>
-      </c>
-      <c r="D111" s="0" t="n">
-        <v>62.47</v>
-      </c>
-      <c r="E111" s="0" t="n">
-        <v>70.4</v>
-      </c>
-      <c r="F111" s="0" t="n">
-        <v>41.55</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B113" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C113" s="0" t="n">
-        <v>71.56</v>
-      </c>
-      <c r="D113" s="0" t="n">
-        <v>69.54</v>
-      </c>
-      <c r="E113" s="0" t="n">
-        <v>65.77</v>
-      </c>
-      <c r="F113" s="0" t="n">
-        <v>79.27</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B114" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C114" s="0" t="n">
-        <v>69.65</v>
-      </c>
-      <c r="D114" s="0" t="n">
-        <v>67.49</v>
-      </c>
-      <c r="E114" s="0" t="n">
-        <v>64.28</v>
-      </c>
-      <c r="F114" s="0" t="n">
-        <v>77.12</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B115" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C115" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D115" s="0" t="n">
-        <v>48.63</v>
-      </c>
-      <c r="E115" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F115" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C116" s="0" t="n">
-        <v>56.76</v>
-      </c>
-      <c r="D116" s="0" t="n">
-        <v>61.37</v>
-      </c>
-      <c r="E116" s="0" t="n">
-        <v>62.93</v>
-      </c>
-      <c r="F116" s="0" t="n">
-        <v>52.57</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B117" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C117" s="0" t="n">
-        <v>55.06</v>
-      </c>
-      <c r="D117" s="0" t="n">
-        <v>63.67</v>
-      </c>
-      <c r="E117" s="0" t="n">
-        <v>70.19</v>
-      </c>
-      <c r="F117" s="0" t="n">
-        <v>46.02</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B119" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C119" s="0" t="n">
-        <v>69.22</v>
-      </c>
-      <c r="D119" s="0" t="n">
-        <v>69.02</v>
-      </c>
-      <c r="E119" s="0" t="n">
-        <v>67.44</v>
-      </c>
-      <c r="F119" s="0" t="n">
-        <v>71.99</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B120" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C120" s="0" t="n">
-        <v>68.99</v>
-      </c>
-      <c r="D120" s="0" t="n">
-        <v>67.3</v>
-      </c>
-      <c r="E120" s="0" t="n">
-        <v>64.56</v>
-      </c>
-      <c r="F120" s="0" t="n">
-        <v>75.25</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B121" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C121" s="0" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="D121" s="0" t="n">
-        <v>48.63</v>
-      </c>
-      <c r="E121" s="0" t="n">
-        <v>3.76</v>
-      </c>
-      <c r="F121" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B122" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C122" s="0" t="n">
-        <v>60.34</v>
-      </c>
-      <c r="D122" s="0" t="n">
-        <v>62.54</v>
-      </c>
-      <c r="E122" s="0" t="n">
-        <v>62.42</v>
-      </c>
-      <c r="F122" s="0" t="n">
-        <v>59.11</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B123" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="0" t="n">
-        <v>60.55</v>
-      </c>
-      <c r="D123" s="0" t="n">
-        <v>65.87</v>
-      </c>
-      <c r="E123" s="0" t="n">
-        <v>69.84</v>
-      </c>
-      <c r="F123" s="0" t="n">
-        <v>54.18</v>
+      <c r="E123" s="3" t="n">
+        <v>69.51</v>
+      </c>
+      <c r="F123" s="3" t="n">
+        <v>65.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added BR - Count Vectorization results for Lucene, Thunderbird, Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-binary-classification/binary-classification-results.xlsx
+++ b/thesis-binary-classification/binary-classification-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="30">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + lem + SMOTE + RUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + tfidf + ngram(3) + stopwords + lemmatization</t>
   </si>
 </sst>
 </file>
@@ -302,15 +308,15 @@
   </sheetPr>
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="A107:F111"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,15 +3010,14 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C119" activeCellId="1" sqref="A107:F111 C119"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B107" activeCellId="0" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,7 +3545,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>68.9</v>
@@ -3560,7 +3565,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>69.32</v>
@@ -3580,7 +3585,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
@@ -3600,7 +3605,7 @@
         <v>10</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>57.61</v>
@@ -3620,7 +3625,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>57.9</v>
@@ -3640,7 +3645,7 @@
         <v>6</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>70.59</v>
@@ -3660,7 +3665,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>69.35</v>
@@ -3680,7 +3685,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>0</v>
@@ -3700,7 +3705,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>58.43</v>
@@ -3720,7 +3725,7 @@
         <v>11</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>60.44</v>
@@ -5106,15 +5111,14 @@
   </sheetPr>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F111" activeCellId="0" sqref="A107:F111"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,7 +5646,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>62.12</v>
@@ -5662,7 +5666,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>63.45</v>
@@ -5682,7 +5686,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>5.47</v>
@@ -5702,7 +5706,7 @@
         <v>10</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>57.44</v>
@@ -5722,7 +5726,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>53.88</v>
@@ -5742,7 +5746,7 @@
         <v>6</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>63.17</v>
@@ -5762,7 +5766,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>63.51</v>
@@ -5782,7 +5786,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>5.47</v>
@@ -5802,7 +5806,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>55.3</v>
@@ -5822,7 +5826,7 @@
         <v>11</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>55.92</v>

</xml_diff>